<commit_message>
cambio en el login
</commit_message>
<xml_diff>
--- a/public/plantillas/productos_plantilla.xlsx
+++ b/public/plantillas/productos_plantilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\work\work\RedNuevaConexion\frontend\public\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBE4CD0-BF70-4CA9-BC52-6689C32713A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D311A32-B168-4E70-89B4-63BACBF77B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3FE219BE-8012-4E43-B72C-AFF1DCF4E483}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Codigo / Serial:</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>Tipo:</t>
-  </si>
-  <si>
-    <t>Stock:</t>
   </si>
   <si>
     <t>Producto</t>
@@ -444,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4717DD0-B11E-49FE-8079-691DA3F6AA0C}">
-  <dimension ref="A1:AB509"/>
+  <dimension ref="A1:AB515"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -484,9 +481,7 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="H1" s="1"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -516,7 +511,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="H2" s="1"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -545,7 +540,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="H3" s="1"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -574,7 +569,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="H4" s="1"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -604,7 +599,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="H5" s="1"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -634,7 +629,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="H6" s="1"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -664,7 +659,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="H7" s="1"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -694,7 +689,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="H8" s="1"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -724,7 +719,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="H9" s="1"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -753,7 +748,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="H10" s="1"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -782,7 +777,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="H11" s="1"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -812,7 +807,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="H12" s="1"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -842,7 +837,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="H13" s="1"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -872,7 +867,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="H14" s="1"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -902,7 +897,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="H15" s="1"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -932,7 +927,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="H16" s="1"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -962,7 +957,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="H17" s="1"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -992,7 +987,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="H18" s="1"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -1022,7 +1017,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="H19" s="1"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -1052,7 +1047,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="H20" s="1"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -1082,7 +1077,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="H21" s="1"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -1112,7 +1107,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="H22" s="1"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -1142,7 +1137,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="H23" s="1"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -1172,7 +1167,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
+      <c r="H24" s="1"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -1202,7 +1197,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
+      <c r="H25" s="1"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -1232,7 +1227,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
+      <c r="H26" s="1"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -1262,7 +1257,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
+      <c r="H27" s="1"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
@@ -1292,7 +1287,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
+      <c r="H28" s="1"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
@@ -1322,7 +1317,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
+      <c r="H29" s="1"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -1352,7 +1347,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
+      <c r="H30" s="1"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -1382,7 +1377,7 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
+      <c r="H31" s="1"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
@@ -1412,7 +1407,7 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
+      <c r="H32" s="1"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
@@ -1442,7 +1437,7 @@
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
+      <c r="H33" s="1"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
@@ -1472,7 +1467,7 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
+      <c r="H34" s="1"/>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
@@ -1502,7 +1497,7 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
+      <c r="H35" s="1"/>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
@@ -1532,7 +1527,7 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
+      <c r="H36" s="1"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
@@ -1562,7 +1557,7 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
+      <c r="H37" s="1"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
@@ -1592,7 +1587,7 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
+      <c r="H38" s="1"/>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
@@ -1622,7 +1617,7 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
+      <c r="H39" s="1"/>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
@@ -1652,7 +1647,7 @@
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
+      <c r="H40" s="1"/>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
@@ -1682,7 +1677,7 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
+      <c r="H41" s="1"/>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
@@ -1712,7 +1707,7 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
+      <c r="H42" s="1"/>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
@@ -1742,7 +1737,7 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
+      <c r="H43" s="1"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
@@ -1772,7 +1767,7 @@
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
+      <c r="H44" s="1"/>
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
@@ -1802,7 +1797,7 @@
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
+      <c r="H45" s="1"/>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
@@ -1832,7 +1827,7 @@
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
+      <c r="H46" s="1"/>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
@@ -1862,7 +1857,7 @@
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
+      <c r="H47" s="1"/>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
@@ -1892,7 +1887,7 @@
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
+      <c r="H48" s="1"/>
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
@@ -1922,7 +1917,7 @@
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
+      <c r="H49" s="1"/>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
@@ -1952,7 +1947,7 @@
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
+      <c r="H50" s="1"/>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
@@ -1982,7 +1977,7 @@
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
+      <c r="H51" s="1"/>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
@@ -2012,7 +2007,7 @@
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
+      <c r="H52" s="1"/>
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
@@ -2042,7 +2037,7 @@
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
+      <c r="H53" s="1"/>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
@@ -2072,7 +2067,7 @@
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
+      <c r="H54" s="1"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
@@ -2102,7 +2097,7 @@
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
+      <c r="H55" s="1"/>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
@@ -2132,7 +2127,7 @@
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
+      <c r="H56" s="1"/>
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
@@ -2162,7 +2157,7 @@
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
+      <c r="H57" s="1"/>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
@@ -2192,7 +2187,7 @@
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
-      <c r="H58" s="2"/>
+      <c r="H58" s="1"/>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
@@ -2222,7 +2217,7 @@
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
+      <c r="H59" s="1"/>
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
@@ -2252,7 +2247,7 @@
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
+      <c r="H60" s="1"/>
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
@@ -2282,7 +2277,7 @@
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
+      <c r="H61" s="1"/>
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
@@ -2312,7 +2307,7 @@
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
-      <c r="H62" s="2"/>
+      <c r="H62" s="1"/>
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
@@ -2342,7 +2337,7 @@
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
+      <c r="H63" s="1"/>
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
@@ -2372,7 +2367,7 @@
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
+      <c r="H64" s="1"/>
       <c r="I64" s="3"/>
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
@@ -2402,7 +2397,7 @@
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
+      <c r="H65" s="1"/>
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
@@ -2432,7 +2427,7 @@
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
+      <c r="H66" s="1"/>
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
@@ -2462,7 +2457,7 @@
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
+      <c r="H67" s="1"/>
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
@@ -2492,7 +2487,7 @@
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
-      <c r="H68" s="2"/>
+      <c r="H68" s="1"/>
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
@@ -2522,7 +2517,7 @@
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
+      <c r="H69" s="1"/>
       <c r="I69" s="3"/>
       <c r="J69" s="3"/>
       <c r="K69" s="3"/>
@@ -2552,7 +2547,7 @@
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
+      <c r="H70" s="1"/>
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
       <c r="K70" s="3"/>
@@ -2582,7 +2577,7 @@
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
-      <c r="H71" s="2"/>
+      <c r="H71" s="1"/>
       <c r="I71" s="3"/>
       <c r="J71" s="3"/>
       <c r="K71" s="3"/>
@@ -2612,7 +2607,7 @@
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
-      <c r="H72" s="2"/>
+      <c r="H72" s="1"/>
       <c r="I72" s="3"/>
       <c r="J72" s="3"/>
       <c r="K72" s="3"/>
@@ -2642,7 +2637,7 @@
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
+      <c r="H73" s="1"/>
       <c r="I73" s="3"/>
       <c r="J73" s="3"/>
       <c r="K73" s="3"/>
@@ -2672,7 +2667,7 @@
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
-      <c r="H74" s="2"/>
+      <c r="H74" s="1"/>
       <c r="I74" s="3"/>
       <c r="J74" s="3"/>
       <c r="K74" s="3"/>
@@ -2702,7 +2697,7 @@
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
-      <c r="H75" s="2"/>
+      <c r="H75" s="1"/>
       <c r="I75" s="3"/>
       <c r="J75" s="3"/>
       <c r="K75" s="3"/>
@@ -2732,7 +2727,7 @@
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
-      <c r="H76" s="2"/>
+      <c r="H76" s="1"/>
       <c r="I76" s="3"/>
       <c r="J76" s="3"/>
       <c r="K76" s="3"/>
@@ -2762,7 +2757,7 @@
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
-      <c r="H77" s="2"/>
+      <c r="H77" s="1"/>
       <c r="I77" s="3"/>
       <c r="J77" s="3"/>
       <c r="K77" s="3"/>
@@ -2792,7 +2787,7 @@
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
-      <c r="H78" s="2"/>
+      <c r="H78" s="1"/>
       <c r="I78" s="3"/>
       <c r="J78" s="3"/>
       <c r="K78" s="3"/>
@@ -2822,7 +2817,7 @@
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
-      <c r="H79" s="2"/>
+      <c r="H79" s="1"/>
       <c r="I79" s="3"/>
       <c r="J79" s="3"/>
       <c r="K79" s="3"/>
@@ -2852,7 +2847,7 @@
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
-      <c r="H80" s="2"/>
+      <c r="H80" s="1"/>
       <c r="I80" s="3"/>
       <c r="J80" s="3"/>
       <c r="K80" s="3"/>
@@ -2882,7 +2877,7 @@
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
-      <c r="H81" s="2"/>
+      <c r="H81" s="1"/>
       <c r="I81" s="3"/>
       <c r="J81" s="3"/>
       <c r="K81" s="3"/>
@@ -2912,7 +2907,7 @@
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
-      <c r="H82" s="2"/>
+      <c r="H82" s="1"/>
       <c r="I82" s="3"/>
       <c r="J82" s="3"/>
       <c r="K82" s="3"/>
@@ -2942,7 +2937,7 @@
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
-      <c r="H83" s="2"/>
+      <c r="H83" s="1"/>
       <c r="I83" s="3"/>
       <c r="J83" s="3"/>
       <c r="K83" s="3"/>
@@ -2972,7 +2967,7 @@
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
-      <c r="H84" s="2"/>
+      <c r="H84" s="1"/>
       <c r="I84" s="3"/>
       <c r="J84" s="3"/>
       <c r="K84" s="3"/>
@@ -3002,7 +2997,7 @@
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
-      <c r="H85" s="2"/>
+      <c r="H85" s="1"/>
       <c r="I85" s="3"/>
       <c r="J85" s="3"/>
       <c r="K85" s="3"/>
@@ -3032,7 +3027,7 @@
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
-      <c r="H86" s="2"/>
+      <c r="H86" s="1"/>
       <c r="I86" s="3"/>
       <c r="J86" s="3"/>
       <c r="K86" s="3"/>
@@ -3062,7 +3057,7 @@
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
-      <c r="H87" s="2"/>
+      <c r="H87" s="1"/>
       <c r="I87" s="3"/>
       <c r="J87" s="3"/>
       <c r="K87" s="3"/>
@@ -3092,7 +3087,7 @@
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
-      <c r="H88" s="2"/>
+      <c r="H88" s="1"/>
       <c r="I88" s="3"/>
       <c r="J88" s="3"/>
       <c r="K88" s="3"/>
@@ -3122,7 +3117,7 @@
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
-      <c r="H89" s="2"/>
+      <c r="H89" s="1"/>
       <c r="I89" s="3"/>
       <c r="J89" s="3"/>
       <c r="K89" s="3"/>
@@ -3152,7 +3147,7 @@
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
-      <c r="H90" s="2"/>
+      <c r="H90" s="1"/>
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
       <c r="K90" s="3"/>
@@ -3182,7 +3177,7 @@
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
-      <c r="H91" s="2"/>
+      <c r="H91" s="1"/>
       <c r="I91" s="3"/>
       <c r="J91" s="3"/>
       <c r="K91" s="3"/>
@@ -3212,7 +3207,7 @@
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
-      <c r="H92" s="2"/>
+      <c r="H92" s="1"/>
       <c r="I92" s="3"/>
       <c r="J92" s="3"/>
       <c r="K92" s="3"/>
@@ -3242,7 +3237,7 @@
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
-      <c r="H93" s="2"/>
+      <c r="H93" s="1"/>
       <c r="I93" s="3"/>
       <c r="J93" s="3"/>
       <c r="K93" s="3"/>
@@ -3272,7 +3267,7 @@
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
-      <c r="H94" s="2"/>
+      <c r="H94" s="1"/>
       <c r="I94" s="3"/>
       <c r="J94" s="3"/>
       <c r="K94" s="3"/>
@@ -3302,7 +3297,7 @@
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
-      <c r="H95" s="2"/>
+      <c r="H95" s="1"/>
       <c r="I95" s="3"/>
       <c r="J95" s="3"/>
       <c r="K95" s="3"/>
@@ -3332,7 +3327,7 @@
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
-      <c r="H96" s="2"/>
+      <c r="H96" s="1"/>
       <c r="I96" s="3"/>
       <c r="J96" s="3"/>
       <c r="K96" s="3"/>
@@ -3362,7 +3357,7 @@
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
-      <c r="H97" s="2"/>
+      <c r="H97" s="1"/>
       <c r="I97" s="3"/>
       <c r="J97" s="3"/>
       <c r="K97" s="3"/>
@@ -3392,7 +3387,7 @@
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
-      <c r="H98" s="2"/>
+      <c r="H98" s="1"/>
       <c r="I98" s="3"/>
       <c r="J98" s="3"/>
       <c r="K98" s="3"/>
@@ -3422,7 +3417,7 @@
       <c r="E99" s="2"/>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
-      <c r="H99" s="2"/>
+      <c r="H99" s="1"/>
       <c r="I99" s="3"/>
       <c r="J99" s="3"/>
       <c r="K99" s="3"/>
@@ -3452,7 +3447,7 @@
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
-      <c r="H100" s="2"/>
+      <c r="H100" s="1"/>
       <c r="I100" s="3"/>
       <c r="J100" s="3"/>
       <c r="K100" s="3"/>
@@ -3482,7 +3477,7 @@
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
-      <c r="H101" s="2"/>
+      <c r="H101" s="1"/>
       <c r="I101" s="3"/>
       <c r="J101" s="3"/>
       <c r="K101" s="3"/>
@@ -3512,7 +3507,7 @@
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
-      <c r="H102" s="2"/>
+      <c r="H102" s="1"/>
       <c r="I102" s="3"/>
       <c r="J102" s="3"/>
       <c r="K102" s="3"/>
@@ -3542,7 +3537,7 @@
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
-      <c r="H103" s="2"/>
+      <c r="H103" s="1"/>
       <c r="I103" s="3"/>
       <c r="J103" s="3"/>
       <c r="K103" s="3"/>
@@ -3572,7 +3567,7 @@
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
       <c r="G104" s="2"/>
-      <c r="H104" s="2"/>
+      <c r="H104" s="1"/>
       <c r="I104" s="3"/>
       <c r="J104" s="3"/>
       <c r="K104" s="3"/>
@@ -3602,7 +3597,7 @@
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
       <c r="G105" s="2"/>
-      <c r="H105" s="2"/>
+      <c r="H105" s="1"/>
       <c r="I105" s="3"/>
       <c r="J105" s="3"/>
       <c r="K105" s="3"/>
@@ -3632,7 +3627,7 @@
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
       <c r="G106" s="2"/>
-      <c r="H106" s="2"/>
+      <c r="H106" s="1"/>
       <c r="I106" s="3"/>
       <c r="J106" s="3"/>
       <c r="K106" s="3"/>
@@ -3662,7 +3657,7 @@
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
       <c r="G107" s="2"/>
-      <c r="H107" s="2"/>
+      <c r="H107" s="1"/>
       <c r="I107" s="3"/>
       <c r="J107" s="3"/>
       <c r="K107" s="3"/>
@@ -3692,7 +3687,7 @@
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
       <c r="G108" s="2"/>
-      <c r="H108" s="2"/>
+      <c r="H108" s="1"/>
       <c r="I108" s="3"/>
       <c r="J108" s="3"/>
       <c r="K108" s="3"/>
@@ -3722,7 +3717,7 @@
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
       <c r="G109" s="2"/>
-      <c r="H109" s="2"/>
+      <c r="H109" s="1"/>
       <c r="I109" s="3"/>
       <c r="J109" s="3"/>
       <c r="K109" s="3"/>
@@ -3752,7 +3747,7 @@
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
       <c r="G110" s="2"/>
-      <c r="H110" s="2"/>
+      <c r="H110" s="1"/>
       <c r="I110" s="3"/>
       <c r="J110" s="3"/>
       <c r="K110" s="3"/>
@@ -3782,7 +3777,7 @@
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
       <c r="G111" s="2"/>
-      <c r="H111" s="2"/>
+      <c r="H111" s="1"/>
       <c r="I111" s="3"/>
       <c r="J111" s="3"/>
       <c r="K111" s="3"/>
@@ -3812,7 +3807,7 @@
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
       <c r="G112" s="2"/>
-      <c r="H112" s="2"/>
+      <c r="H112" s="1"/>
       <c r="I112" s="3"/>
       <c r="J112" s="3"/>
       <c r="K112" s="3"/>
@@ -3842,7 +3837,7 @@
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
       <c r="G113" s="2"/>
-      <c r="H113" s="2"/>
+      <c r="H113" s="1"/>
       <c r="I113" s="3"/>
       <c r="J113" s="3"/>
       <c r="K113" s="3"/>
@@ -3872,7 +3867,7 @@
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
       <c r="G114" s="2"/>
-      <c r="H114" s="2"/>
+      <c r="H114" s="1"/>
       <c r="I114" s="3"/>
       <c r="J114" s="3"/>
       <c r="K114" s="3"/>
@@ -3902,7 +3897,7 @@
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
       <c r="G115" s="2"/>
-      <c r="H115" s="2"/>
+      <c r="H115" s="1"/>
       <c r="I115" s="3"/>
       <c r="J115" s="3"/>
       <c r="K115" s="3"/>
@@ -3932,7 +3927,7 @@
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
       <c r="G116" s="2"/>
-      <c r="H116" s="2"/>
+      <c r="H116" s="1"/>
       <c r="I116" s="3"/>
       <c r="J116" s="3"/>
       <c r="K116" s="3"/>
@@ -3962,7 +3957,7 @@
       <c r="E117" s="2"/>
       <c r="F117" s="2"/>
       <c r="G117" s="2"/>
-      <c r="H117" s="2"/>
+      <c r="H117" s="1"/>
       <c r="I117" s="3"/>
       <c r="J117" s="3"/>
       <c r="K117" s="3"/>
@@ -3992,7 +3987,7 @@
       <c r="E118" s="2"/>
       <c r="F118" s="2"/>
       <c r="G118" s="2"/>
-      <c r="H118" s="2"/>
+      <c r="H118" s="1"/>
       <c r="I118" s="3"/>
       <c r="J118" s="3"/>
       <c r="K118" s="3"/>
@@ -4022,7 +4017,7 @@
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
       <c r="G119" s="2"/>
-      <c r="H119" s="2"/>
+      <c r="H119" s="1"/>
       <c r="I119" s="3"/>
       <c r="J119" s="3"/>
       <c r="K119" s="3"/>
@@ -4052,7 +4047,7 @@
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
       <c r="G120" s="2"/>
-      <c r="H120" s="2"/>
+      <c r="H120" s="1"/>
       <c r="I120" s="3"/>
       <c r="J120" s="3"/>
       <c r="K120" s="3"/>
@@ -4082,7 +4077,7 @@
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
       <c r="G121" s="2"/>
-      <c r="H121" s="2"/>
+      <c r="H121" s="1"/>
       <c r="I121" s="3"/>
       <c r="J121" s="3"/>
       <c r="K121" s="3"/>
@@ -4112,7 +4107,7 @@
       <c r="E122" s="2"/>
       <c r="F122" s="2"/>
       <c r="G122" s="2"/>
-      <c r="H122" s="2"/>
+      <c r="H122" s="1"/>
       <c r="I122" s="3"/>
       <c r="J122" s="3"/>
       <c r="K122" s="3"/>
@@ -4142,7 +4137,7 @@
       <c r="E123" s="2"/>
       <c r="F123" s="2"/>
       <c r="G123" s="2"/>
-      <c r="H123" s="2"/>
+      <c r="H123" s="1"/>
       <c r="I123" s="3"/>
       <c r="J123" s="3"/>
       <c r="K123" s="3"/>
@@ -4172,7 +4167,7 @@
       <c r="E124" s="2"/>
       <c r="F124" s="2"/>
       <c r="G124" s="2"/>
-      <c r="H124" s="2"/>
+      <c r="H124" s="1"/>
       <c r="I124" s="3"/>
       <c r="J124" s="3"/>
       <c r="K124" s="3"/>
@@ -4202,7 +4197,7 @@
       <c r="E125" s="2"/>
       <c r="F125" s="2"/>
       <c r="G125" s="2"/>
-      <c r="H125" s="2"/>
+      <c r="H125" s="1"/>
       <c r="I125" s="3"/>
       <c r="J125" s="3"/>
       <c r="K125" s="3"/>
@@ -4232,7 +4227,7 @@
       <c r="E126" s="2"/>
       <c r="F126" s="2"/>
       <c r="G126" s="2"/>
-      <c r="H126" s="2"/>
+      <c r="H126" s="1"/>
       <c r="I126" s="3"/>
       <c r="J126" s="3"/>
       <c r="K126" s="3"/>
@@ -4262,7 +4257,7 @@
       <c r="E127" s="2"/>
       <c r="F127" s="2"/>
       <c r="G127" s="2"/>
-      <c r="H127" s="2"/>
+      <c r="H127" s="1"/>
       <c r="I127" s="3"/>
       <c r="J127" s="3"/>
       <c r="K127" s="3"/>
@@ -4292,7 +4287,7 @@
       <c r="E128" s="2"/>
       <c r="F128" s="2"/>
       <c r="G128" s="2"/>
-      <c r="H128" s="2"/>
+      <c r="H128" s="1"/>
       <c r="I128" s="3"/>
       <c r="J128" s="3"/>
       <c r="K128" s="3"/>
@@ -4322,7 +4317,7 @@
       <c r="E129" s="2"/>
       <c r="F129" s="2"/>
       <c r="G129" s="2"/>
-      <c r="H129" s="2"/>
+      <c r="H129" s="1"/>
       <c r="I129" s="3"/>
       <c r="J129" s="3"/>
       <c r="K129" s="3"/>
@@ -4352,7 +4347,7 @@
       <c r="E130" s="2"/>
       <c r="F130" s="2"/>
       <c r="G130" s="2"/>
-      <c r="H130" s="2"/>
+      <c r="H130" s="1"/>
       <c r="I130" s="3"/>
       <c r="J130" s="3"/>
       <c r="K130" s="3"/>
@@ -4382,7 +4377,7 @@
       <c r="E131" s="2"/>
       <c r="F131" s="2"/>
       <c r="G131" s="2"/>
-      <c r="H131" s="2"/>
+      <c r="H131" s="1"/>
       <c r="I131" s="3"/>
       <c r="J131" s="3"/>
       <c r="K131" s="3"/>
@@ -4412,7 +4407,7 @@
       <c r="E132" s="2"/>
       <c r="F132" s="2"/>
       <c r="G132" s="2"/>
-      <c r="H132" s="2"/>
+      <c r="H132" s="1"/>
       <c r="I132" s="3"/>
       <c r="J132" s="3"/>
       <c r="K132" s="3"/>
@@ -4442,7 +4437,7 @@
       <c r="E133" s="2"/>
       <c r="F133" s="2"/>
       <c r="G133" s="2"/>
-      <c r="H133" s="2"/>
+      <c r="H133" s="1"/>
       <c r="I133" s="3"/>
       <c r="J133" s="3"/>
       <c r="K133" s="3"/>
@@ -4472,7 +4467,7 @@
       <c r="E134" s="2"/>
       <c r="F134" s="2"/>
       <c r="G134" s="2"/>
-      <c r="H134" s="2"/>
+      <c r="H134" s="1"/>
       <c r="I134" s="3"/>
       <c r="J134" s="3"/>
       <c r="K134" s="3"/>
@@ -4502,7 +4497,7 @@
       <c r="E135" s="2"/>
       <c r="F135" s="2"/>
       <c r="G135" s="2"/>
-      <c r="H135" s="2"/>
+      <c r="H135" s="1"/>
       <c r="I135" s="3"/>
       <c r="J135" s="3"/>
       <c r="K135" s="3"/>
@@ -4532,7 +4527,7 @@
       <c r="E136" s="2"/>
       <c r="F136" s="2"/>
       <c r="G136" s="2"/>
-      <c r="H136" s="2"/>
+      <c r="H136" s="1"/>
       <c r="I136" s="3"/>
       <c r="J136" s="3"/>
       <c r="K136" s="3"/>
@@ -4562,7 +4557,7 @@
       <c r="E137" s="2"/>
       <c r="F137" s="2"/>
       <c r="G137" s="2"/>
-      <c r="H137" s="2"/>
+      <c r="H137" s="1"/>
       <c r="I137" s="3"/>
       <c r="J137" s="3"/>
       <c r="K137" s="3"/>
@@ -4592,7 +4587,7 @@
       <c r="E138" s="2"/>
       <c r="F138" s="2"/>
       <c r="G138" s="2"/>
-      <c r="H138" s="2"/>
+      <c r="H138" s="1"/>
       <c r="I138" s="3"/>
       <c r="J138" s="3"/>
       <c r="K138" s="3"/>
@@ -4622,7 +4617,7 @@
       <c r="E139" s="2"/>
       <c r="F139" s="2"/>
       <c r="G139" s="2"/>
-      <c r="H139" s="2"/>
+      <c r="H139" s="1"/>
       <c r="I139" s="3"/>
       <c r="J139" s="3"/>
       <c r="K139" s="3"/>
@@ -4652,7 +4647,7 @@
       <c r="E140" s="2"/>
       <c r="F140" s="2"/>
       <c r="G140" s="2"/>
-      <c r="H140" s="2"/>
+      <c r="H140" s="1"/>
       <c r="I140" s="3"/>
       <c r="J140" s="3"/>
       <c r="K140" s="3"/>
@@ -4682,7 +4677,7 @@
       <c r="E141" s="2"/>
       <c r="F141" s="2"/>
       <c r="G141" s="2"/>
-      <c r="H141" s="2"/>
+      <c r="H141" s="1"/>
       <c r="I141" s="3"/>
       <c r="J141" s="3"/>
       <c r="K141" s="3"/>
@@ -4712,7 +4707,7 @@
       <c r="E142" s="2"/>
       <c r="F142" s="2"/>
       <c r="G142" s="2"/>
-      <c r="H142" s="2"/>
+      <c r="H142" s="1"/>
       <c r="I142" s="3"/>
       <c r="J142" s="3"/>
       <c r="K142" s="3"/>
@@ -4742,7 +4737,7 @@
       <c r="E143" s="2"/>
       <c r="F143" s="2"/>
       <c r="G143" s="2"/>
-      <c r="H143" s="2"/>
+      <c r="H143" s="1"/>
       <c r="I143" s="3"/>
       <c r="J143" s="3"/>
       <c r="K143" s="3"/>
@@ -4772,7 +4767,7 @@
       <c r="E144" s="2"/>
       <c r="F144" s="2"/>
       <c r="G144" s="2"/>
-      <c r="H144" s="2"/>
+      <c r="H144" s="1"/>
       <c r="I144" s="3"/>
       <c r="J144" s="3"/>
       <c r="K144" s="3"/>
@@ -4802,7 +4797,7 @@
       <c r="E145" s="2"/>
       <c r="F145" s="2"/>
       <c r="G145" s="2"/>
-      <c r="H145" s="2"/>
+      <c r="H145" s="1"/>
       <c r="I145" s="3"/>
       <c r="J145" s="3"/>
       <c r="K145" s="3"/>
@@ -4832,7 +4827,7 @@
       <c r="E146" s="2"/>
       <c r="F146" s="2"/>
       <c r="G146" s="2"/>
-      <c r="H146" s="2"/>
+      <c r="H146" s="1"/>
       <c r="I146" s="3"/>
       <c r="J146" s="3"/>
       <c r="K146" s="3"/>
@@ -4862,7 +4857,7 @@
       <c r="E147" s="2"/>
       <c r="F147" s="2"/>
       <c r="G147" s="2"/>
-      <c r="H147" s="2"/>
+      <c r="H147" s="1"/>
       <c r="I147" s="3"/>
       <c r="J147" s="3"/>
       <c r="K147" s="3"/>
@@ -4892,7 +4887,7 @@
       <c r="E148" s="2"/>
       <c r="F148" s="2"/>
       <c r="G148" s="2"/>
-      <c r="H148" s="2"/>
+      <c r="H148" s="1"/>
       <c r="I148" s="3"/>
       <c r="J148" s="3"/>
       <c r="K148" s="3"/>
@@ -4922,7 +4917,7 @@
       <c r="E149" s="2"/>
       <c r="F149" s="2"/>
       <c r="G149" s="2"/>
-      <c r="H149" s="2"/>
+      <c r="H149" s="1"/>
       <c r="I149" s="3"/>
       <c r="J149" s="3"/>
       <c r="K149" s="3"/>
@@ -4952,7 +4947,7 @@
       <c r="E150" s="2"/>
       <c r="F150" s="2"/>
       <c r="G150" s="2"/>
-      <c r="H150" s="2"/>
+      <c r="H150" s="1"/>
       <c r="I150" s="3"/>
       <c r="J150" s="3"/>
       <c r="K150" s="3"/>
@@ -4982,7 +4977,7 @@
       <c r="E151" s="2"/>
       <c r="F151" s="2"/>
       <c r="G151" s="2"/>
-      <c r="H151" s="2"/>
+      <c r="H151" s="1"/>
       <c r="I151" s="3"/>
       <c r="J151" s="3"/>
       <c r="K151" s="3"/>
@@ -5012,7 +5007,7 @@
       <c r="E152" s="2"/>
       <c r="F152" s="2"/>
       <c r="G152" s="2"/>
-      <c r="H152" s="2"/>
+      <c r="H152" s="1"/>
       <c r="I152" s="3"/>
       <c r="J152" s="3"/>
       <c r="K152" s="3"/>
@@ -5042,7 +5037,7 @@
       <c r="E153" s="2"/>
       <c r="F153" s="2"/>
       <c r="G153" s="2"/>
-      <c r="H153" s="2"/>
+      <c r="H153" s="1"/>
       <c r="I153" s="3"/>
       <c r="J153" s="3"/>
       <c r="K153" s="3"/>
@@ -5072,7 +5067,7 @@
       <c r="E154" s="2"/>
       <c r="F154" s="2"/>
       <c r="G154" s="2"/>
-      <c r="H154" s="2"/>
+      <c r="H154" s="1"/>
       <c r="I154" s="3"/>
       <c r="J154" s="3"/>
       <c r="K154" s="3"/>
@@ -5102,7 +5097,7 @@
       <c r="E155" s="2"/>
       <c r="F155" s="2"/>
       <c r="G155" s="2"/>
-      <c r="H155" s="2"/>
+      <c r="H155" s="1"/>
       <c r="I155" s="3"/>
       <c r="J155" s="3"/>
       <c r="K155" s="3"/>
@@ -5132,7 +5127,7 @@
       <c r="E156" s="2"/>
       <c r="F156" s="2"/>
       <c r="G156" s="2"/>
-      <c r="H156" s="2"/>
+      <c r="H156" s="1"/>
       <c r="I156" s="3"/>
       <c r="J156" s="3"/>
       <c r="K156" s="3"/>
@@ -5162,7 +5157,7 @@
       <c r="E157" s="2"/>
       <c r="F157" s="2"/>
       <c r="G157" s="2"/>
-      <c r="H157" s="2"/>
+      <c r="H157" s="1"/>
       <c r="I157" s="3"/>
       <c r="J157" s="3"/>
       <c r="K157" s="3"/>
@@ -5192,7 +5187,7 @@
       <c r="E158" s="2"/>
       <c r="F158" s="2"/>
       <c r="G158" s="2"/>
-      <c r="H158" s="2"/>
+      <c r="H158" s="1"/>
       <c r="I158" s="3"/>
       <c r="J158" s="3"/>
       <c r="K158" s="3"/>
@@ -5222,7 +5217,7 @@
       <c r="E159" s="2"/>
       <c r="F159" s="2"/>
       <c r="G159" s="2"/>
-      <c r="H159" s="2"/>
+      <c r="H159" s="1"/>
       <c r="I159" s="3"/>
       <c r="J159" s="3"/>
       <c r="K159" s="3"/>
@@ -5252,7 +5247,7 @@
       <c r="E160" s="2"/>
       <c r="F160" s="2"/>
       <c r="G160" s="2"/>
-      <c r="H160" s="2"/>
+      <c r="H160" s="1"/>
       <c r="I160" s="3"/>
       <c r="J160" s="3"/>
       <c r="K160" s="3"/>
@@ -5282,7 +5277,7 @@
       <c r="E161" s="2"/>
       <c r="F161" s="2"/>
       <c r="G161" s="2"/>
-      <c r="H161" s="2"/>
+      <c r="H161" s="1"/>
       <c r="I161" s="3"/>
       <c r="J161" s="3"/>
       <c r="K161" s="3"/>
@@ -5312,7 +5307,7 @@
       <c r="E162" s="2"/>
       <c r="F162" s="2"/>
       <c r="G162" s="2"/>
-      <c r="H162" s="2"/>
+      <c r="H162" s="1"/>
       <c r="I162" s="3"/>
       <c r="J162" s="3"/>
       <c r="K162" s="3"/>
@@ -5342,7 +5337,7 @@
       <c r="E163" s="2"/>
       <c r="F163" s="2"/>
       <c r="G163" s="2"/>
-      <c r="H163" s="2"/>
+      <c r="H163" s="1"/>
       <c r="I163" s="3"/>
       <c r="J163" s="3"/>
       <c r="K163" s="3"/>
@@ -5372,7 +5367,7 @@
       <c r="E164" s="2"/>
       <c r="F164" s="2"/>
       <c r="G164" s="2"/>
-      <c r="H164" s="2"/>
+      <c r="H164" s="1"/>
       <c r="I164" s="3"/>
       <c r="J164" s="3"/>
       <c r="K164" s="3"/>
@@ -5402,7 +5397,7 @@
       <c r="E165" s="2"/>
       <c r="F165" s="2"/>
       <c r="G165" s="2"/>
-      <c r="H165" s="2"/>
+      <c r="H165" s="1"/>
       <c r="I165" s="3"/>
       <c r="J165" s="3"/>
       <c r="K165" s="3"/>
@@ -5432,7 +5427,7 @@
       <c r="E166" s="2"/>
       <c r="F166" s="2"/>
       <c r="G166" s="2"/>
-      <c r="H166" s="2"/>
+      <c r="H166" s="1"/>
       <c r="I166" s="3"/>
       <c r="J166" s="3"/>
       <c r="K166" s="3"/>
@@ -5462,7 +5457,7 @@
       <c r="E167" s="2"/>
       <c r="F167" s="2"/>
       <c r="G167" s="2"/>
-      <c r="H167" s="2"/>
+      <c r="H167" s="1"/>
       <c r="I167" s="3"/>
       <c r="J167" s="3"/>
       <c r="K167" s="3"/>
@@ -5492,7 +5487,7 @@
       <c r="E168" s="2"/>
       <c r="F168" s="2"/>
       <c r="G168" s="2"/>
-      <c r="H168" s="2"/>
+      <c r="H168" s="1"/>
       <c r="I168" s="3"/>
       <c r="J168" s="3"/>
       <c r="K168" s="3"/>
@@ -5522,7 +5517,7 @@
       <c r="E169" s="2"/>
       <c r="F169" s="2"/>
       <c r="G169" s="2"/>
-      <c r="H169" s="2"/>
+      <c r="H169" s="1"/>
       <c r="I169" s="3"/>
       <c r="J169" s="3"/>
       <c r="K169" s="3"/>
@@ -5552,7 +5547,7 @@
       <c r="E170" s="2"/>
       <c r="F170" s="2"/>
       <c r="G170" s="2"/>
-      <c r="H170" s="2"/>
+      <c r="H170" s="1"/>
       <c r="I170" s="3"/>
       <c r="J170" s="3"/>
       <c r="K170" s="3"/>
@@ -5582,7 +5577,7 @@
       <c r="E171" s="2"/>
       <c r="F171" s="2"/>
       <c r="G171" s="2"/>
-      <c r="H171" s="2"/>
+      <c r="H171" s="1"/>
       <c r="I171" s="3"/>
       <c r="J171" s="3"/>
       <c r="K171" s="3"/>
@@ -5612,7 +5607,7 @@
       <c r="E172" s="2"/>
       <c r="F172" s="2"/>
       <c r="G172" s="2"/>
-      <c r="H172" s="2"/>
+      <c r="H172" s="1"/>
       <c r="I172" s="3"/>
       <c r="J172" s="3"/>
       <c r="K172" s="3"/>
@@ -5642,7 +5637,7 @@
       <c r="E173" s="2"/>
       <c r="F173" s="2"/>
       <c r="G173" s="2"/>
-      <c r="H173" s="2"/>
+      <c r="H173" s="1"/>
       <c r="I173" s="3"/>
       <c r="J173" s="3"/>
       <c r="K173" s="3"/>
@@ -5672,7 +5667,7 @@
       <c r="E174" s="2"/>
       <c r="F174" s="2"/>
       <c r="G174" s="2"/>
-      <c r="H174" s="2"/>
+      <c r="H174" s="1"/>
       <c r="I174" s="3"/>
       <c r="J174" s="3"/>
       <c r="K174" s="3"/>
@@ -5702,7 +5697,7 @@
       <c r="E175" s="2"/>
       <c r="F175" s="2"/>
       <c r="G175" s="2"/>
-      <c r="H175" s="2"/>
+      <c r="H175" s="1"/>
       <c r="I175" s="3"/>
       <c r="J175" s="3"/>
       <c r="K175" s="3"/>
@@ -5732,7 +5727,7 @@
       <c r="E176" s="2"/>
       <c r="F176" s="2"/>
       <c r="G176" s="2"/>
-      <c r="H176" s="2"/>
+      <c r="H176" s="1"/>
       <c r="I176" s="3"/>
       <c r="J176" s="3"/>
       <c r="K176" s="3"/>
@@ -5762,7 +5757,7 @@
       <c r="E177" s="2"/>
       <c r="F177" s="2"/>
       <c r="G177" s="2"/>
-      <c r="H177" s="2"/>
+      <c r="H177" s="1"/>
       <c r="I177" s="3"/>
       <c r="J177" s="3"/>
       <c r="K177" s="3"/>
@@ -5792,7 +5787,7 @@
       <c r="E178" s="2"/>
       <c r="F178" s="2"/>
       <c r="G178" s="2"/>
-      <c r="H178" s="2"/>
+      <c r="H178" s="1"/>
       <c r="I178" s="3"/>
       <c r="J178" s="3"/>
       <c r="K178" s="3"/>
@@ -5822,7 +5817,7 @@
       <c r="E179" s="2"/>
       <c r="F179" s="2"/>
       <c r="G179" s="2"/>
-      <c r="H179" s="2"/>
+      <c r="H179" s="1"/>
       <c r="I179" s="3"/>
       <c r="J179" s="3"/>
       <c r="K179" s="3"/>
@@ -5852,7 +5847,7 @@
       <c r="E180" s="2"/>
       <c r="F180" s="2"/>
       <c r="G180" s="2"/>
-      <c r="H180" s="2"/>
+      <c r="H180" s="1"/>
       <c r="I180" s="3"/>
       <c r="J180" s="3"/>
       <c r="K180" s="3"/>
@@ -5882,7 +5877,7 @@
       <c r="E181" s="2"/>
       <c r="F181" s="2"/>
       <c r="G181" s="2"/>
-      <c r="H181" s="2"/>
+      <c r="H181" s="1"/>
       <c r="I181" s="3"/>
       <c r="J181" s="3"/>
       <c r="K181" s="3"/>
@@ -5912,7 +5907,7 @@
       <c r="E182" s="2"/>
       <c r="F182" s="2"/>
       <c r="G182" s="2"/>
-      <c r="H182" s="2"/>
+      <c r="H182" s="1"/>
       <c r="I182" s="3"/>
       <c r="J182" s="3"/>
       <c r="K182" s="3"/>
@@ -5942,7 +5937,7 @@
       <c r="E183" s="2"/>
       <c r="F183" s="2"/>
       <c r="G183" s="2"/>
-      <c r="H183" s="2"/>
+      <c r="H183" s="1"/>
       <c r="I183" s="3"/>
       <c r="J183" s="3"/>
       <c r="K183" s="3"/>
@@ -5972,7 +5967,7 @@
       <c r="E184" s="2"/>
       <c r="F184" s="2"/>
       <c r="G184" s="2"/>
-      <c r="H184" s="2"/>
+      <c r="H184" s="1"/>
       <c r="I184" s="3"/>
       <c r="J184" s="3"/>
       <c r="K184" s="3"/>
@@ -6002,7 +5997,7 @@
       <c r="E185" s="2"/>
       <c r="F185" s="2"/>
       <c r="G185" s="2"/>
-      <c r="H185" s="2"/>
+      <c r="H185" s="1"/>
       <c r="I185" s="3"/>
       <c r="J185" s="3"/>
       <c r="K185" s="3"/>
@@ -6032,7 +6027,7 @@
       <c r="E186" s="2"/>
       <c r="F186" s="2"/>
       <c r="G186" s="2"/>
-      <c r="H186" s="2"/>
+      <c r="H186" s="1"/>
       <c r="I186" s="3"/>
       <c r="J186" s="3"/>
       <c r="K186" s="3"/>
@@ -6062,7 +6057,7 @@
       <c r="E187" s="2"/>
       <c r="F187" s="2"/>
       <c r="G187" s="2"/>
-      <c r="H187" s="2"/>
+      <c r="H187" s="1"/>
       <c r="I187" s="3"/>
       <c r="J187" s="3"/>
       <c r="K187" s="3"/>
@@ -6092,7 +6087,7 @@
       <c r="E188" s="2"/>
       <c r="F188" s="2"/>
       <c r="G188" s="2"/>
-      <c r="H188" s="2"/>
+      <c r="H188" s="1"/>
       <c r="I188" s="3"/>
       <c r="J188" s="3"/>
       <c r="K188" s="3"/>
@@ -6122,7 +6117,7 @@
       <c r="E189" s="2"/>
       <c r="F189" s="2"/>
       <c r="G189" s="2"/>
-      <c r="H189" s="2"/>
+      <c r="H189" s="1"/>
       <c r="I189" s="3"/>
       <c r="J189" s="3"/>
       <c r="K189" s="3"/>
@@ -6152,7 +6147,7 @@
       <c r="E190" s="2"/>
       <c r="F190" s="2"/>
       <c r="G190" s="2"/>
-      <c r="H190" s="2"/>
+      <c r="H190" s="1"/>
       <c r="I190" s="3"/>
       <c r="J190" s="3"/>
       <c r="K190" s="3"/>
@@ -6182,7 +6177,7 @@
       <c r="E191" s="2"/>
       <c r="F191" s="2"/>
       <c r="G191" s="2"/>
-      <c r="H191" s="2"/>
+      <c r="H191" s="1"/>
       <c r="I191" s="3"/>
       <c r="J191" s="3"/>
       <c r="K191" s="3"/>
@@ -6212,7 +6207,7 @@
       <c r="E192" s="2"/>
       <c r="F192" s="2"/>
       <c r="G192" s="2"/>
-      <c r="H192" s="2"/>
+      <c r="H192" s="1"/>
       <c r="I192" s="3"/>
       <c r="J192" s="3"/>
       <c r="K192" s="3"/>
@@ -6242,7 +6237,7 @@
       <c r="E193" s="2"/>
       <c r="F193" s="2"/>
       <c r="G193" s="2"/>
-      <c r="H193" s="2"/>
+      <c r="H193" s="1"/>
       <c r="I193" s="3"/>
       <c r="J193" s="3"/>
       <c r="K193" s="3"/>
@@ -6272,7 +6267,7 @@
       <c r="E194" s="2"/>
       <c r="F194" s="2"/>
       <c r="G194" s="2"/>
-      <c r="H194" s="2"/>
+      <c r="H194" s="1"/>
       <c r="I194" s="3"/>
       <c r="J194" s="3"/>
       <c r="K194" s="3"/>
@@ -6302,7 +6297,7 @@
       <c r="E195" s="2"/>
       <c r="F195" s="2"/>
       <c r="G195" s="2"/>
-      <c r="H195" s="2"/>
+      <c r="H195" s="1"/>
       <c r="I195" s="3"/>
       <c r="J195" s="3"/>
       <c r="K195" s="3"/>
@@ -6332,7 +6327,7 @@
       <c r="E196" s="2"/>
       <c r="F196" s="2"/>
       <c r="G196" s="2"/>
-      <c r="H196" s="2"/>
+      <c r="H196" s="1"/>
       <c r="I196" s="3"/>
       <c r="J196" s="3"/>
       <c r="K196" s="3"/>
@@ -6362,7 +6357,7 @@
       <c r="E197" s="2"/>
       <c r="F197" s="2"/>
       <c r="G197" s="2"/>
-      <c r="H197" s="2"/>
+      <c r="H197" s="1"/>
       <c r="I197" s="3"/>
       <c r="J197" s="3"/>
       <c r="K197" s="3"/>
@@ -6392,7 +6387,7 @@
       <c r="E198" s="2"/>
       <c r="F198" s="2"/>
       <c r="G198" s="2"/>
-      <c r="H198" s="2"/>
+      <c r="H198" s="1"/>
       <c r="I198" s="3"/>
       <c r="J198" s="3"/>
       <c r="K198" s="3"/>
@@ -6422,7 +6417,7 @@
       <c r="E199" s="2"/>
       <c r="F199" s="2"/>
       <c r="G199" s="2"/>
-      <c r="H199" s="2"/>
+      <c r="H199" s="1"/>
       <c r="I199" s="3"/>
       <c r="J199" s="3"/>
       <c r="K199" s="3"/>
@@ -6452,7 +6447,7 @@
       <c r="E200" s="2"/>
       <c r="F200" s="2"/>
       <c r="G200" s="2"/>
-      <c r="H200" s="2"/>
+      <c r="H200" s="1"/>
       <c r="I200" s="3"/>
       <c r="J200" s="3"/>
       <c r="K200" s="3"/>
@@ -6482,7 +6477,7 @@
       <c r="E201" s="2"/>
       <c r="F201" s="2"/>
       <c r="G201" s="2"/>
-      <c r="H201" s="2"/>
+      <c r="H201" s="1"/>
       <c r="I201" s="3"/>
       <c r="J201" s="3"/>
       <c r="K201" s="3"/>
@@ -6512,7 +6507,7 @@
       <c r="E202" s="2"/>
       <c r="F202" s="2"/>
       <c r="G202" s="2"/>
-      <c r="H202" s="2"/>
+      <c r="H202" s="1"/>
       <c r="I202" s="3"/>
       <c r="J202" s="3"/>
       <c r="K202" s="3"/>
@@ -6542,7 +6537,7 @@
       <c r="E203" s="2"/>
       <c r="F203" s="2"/>
       <c r="G203" s="2"/>
-      <c r="H203" s="2"/>
+      <c r="H203" s="1"/>
       <c r="I203" s="3"/>
       <c r="J203" s="3"/>
       <c r="K203" s="3"/>
@@ -6572,7 +6567,7 @@
       <c r="E204" s="2"/>
       <c r="F204" s="2"/>
       <c r="G204" s="2"/>
-      <c r="H204" s="2"/>
+      <c r="H204" s="1"/>
       <c r="I204" s="3"/>
       <c r="J204" s="3"/>
       <c r="K204" s="3"/>
@@ -6602,7 +6597,7 @@
       <c r="E205" s="2"/>
       <c r="F205" s="2"/>
       <c r="G205" s="2"/>
-      <c r="H205" s="2"/>
+      <c r="H205" s="1"/>
       <c r="I205" s="3"/>
       <c r="J205" s="3"/>
       <c r="K205" s="3"/>
@@ -6632,7 +6627,7 @@
       <c r="E206" s="2"/>
       <c r="F206" s="2"/>
       <c r="G206" s="2"/>
-      <c r="H206" s="2"/>
+      <c r="H206" s="1"/>
       <c r="I206" s="3"/>
       <c r="J206" s="3"/>
       <c r="K206" s="3"/>
@@ -6662,7 +6657,7 @@
       <c r="E207" s="2"/>
       <c r="F207" s="2"/>
       <c r="G207" s="2"/>
-      <c r="H207" s="2"/>
+      <c r="H207" s="1"/>
       <c r="I207" s="3"/>
       <c r="J207" s="3"/>
       <c r="K207" s="3"/>
@@ -6692,7 +6687,7 @@
       <c r="E208" s="2"/>
       <c r="F208" s="2"/>
       <c r="G208" s="2"/>
-      <c r="H208" s="2"/>
+      <c r="H208" s="1"/>
       <c r="I208" s="3"/>
       <c r="J208" s="3"/>
       <c r="K208" s="3"/>
@@ -6722,7 +6717,7 @@
       <c r="E209" s="2"/>
       <c r="F209" s="2"/>
       <c r="G209" s="2"/>
-      <c r="H209" s="2"/>
+      <c r="H209" s="1"/>
       <c r="I209" s="3"/>
       <c r="J209" s="3"/>
       <c r="K209" s="3"/>
@@ -6752,7 +6747,7 @@
       <c r="E210" s="2"/>
       <c r="F210" s="2"/>
       <c r="G210" s="2"/>
-      <c r="H210" s="2"/>
+      <c r="H210" s="1"/>
       <c r="I210" s="3"/>
       <c r="J210" s="3"/>
       <c r="K210" s="3"/>
@@ -6782,7 +6777,7 @@
       <c r="E211" s="2"/>
       <c r="F211" s="2"/>
       <c r="G211" s="2"/>
-      <c r="H211" s="2"/>
+      <c r="H211" s="1"/>
       <c r="I211" s="3"/>
       <c r="J211" s="3"/>
       <c r="K211" s="3"/>
@@ -6812,7 +6807,7 @@
       <c r="E212" s="2"/>
       <c r="F212" s="2"/>
       <c r="G212" s="2"/>
-      <c r="H212" s="2"/>
+      <c r="H212" s="1"/>
       <c r="I212" s="3"/>
       <c r="J212" s="3"/>
       <c r="K212" s="3"/>
@@ -6842,7 +6837,7 @@
       <c r="E213" s="2"/>
       <c r="F213" s="2"/>
       <c r="G213" s="2"/>
-      <c r="H213" s="2"/>
+      <c r="H213" s="1"/>
       <c r="I213" s="3"/>
       <c r="J213" s="3"/>
       <c r="K213" s="3"/>
@@ -6872,7 +6867,7 @@
       <c r="E214" s="2"/>
       <c r="F214" s="2"/>
       <c r="G214" s="2"/>
-      <c r="H214" s="2"/>
+      <c r="H214" s="1"/>
       <c r="I214" s="3"/>
       <c r="J214" s="3"/>
       <c r="K214" s="3"/>
@@ -6902,7 +6897,7 @@
       <c r="E215" s="2"/>
       <c r="F215" s="2"/>
       <c r="G215" s="2"/>
-      <c r="H215" s="2"/>
+      <c r="H215" s="1"/>
       <c r="I215" s="3"/>
       <c r="J215" s="3"/>
       <c r="K215" s="3"/>
@@ -6932,7 +6927,7 @@
       <c r="E216" s="2"/>
       <c r="F216" s="2"/>
       <c r="G216" s="2"/>
-      <c r="H216" s="2"/>
+      <c r="H216" s="1"/>
       <c r="I216" s="3"/>
       <c r="J216" s="3"/>
       <c r="K216" s="3"/>
@@ -6962,7 +6957,7 @@
       <c r="E217" s="2"/>
       <c r="F217" s="2"/>
       <c r="G217" s="2"/>
-      <c r="H217" s="2"/>
+      <c r="H217" s="1"/>
       <c r="I217" s="3"/>
       <c r="J217" s="3"/>
       <c r="K217" s="3"/>
@@ -6992,7 +6987,7 @@
       <c r="E218" s="2"/>
       <c r="F218" s="2"/>
       <c r="G218" s="2"/>
-      <c r="H218" s="2"/>
+      <c r="H218" s="1"/>
       <c r="I218" s="3"/>
       <c r="J218" s="3"/>
       <c r="K218" s="3"/>
@@ -7022,7 +7017,7 @@
       <c r="E219" s="2"/>
       <c r="F219" s="2"/>
       <c r="G219" s="2"/>
-      <c r="H219" s="2"/>
+      <c r="H219" s="1"/>
       <c r="I219" s="3"/>
       <c r="J219" s="3"/>
       <c r="K219" s="3"/>
@@ -7052,7 +7047,7 @@
       <c r="E220" s="2"/>
       <c r="F220" s="2"/>
       <c r="G220" s="2"/>
-      <c r="H220" s="2"/>
+      <c r="H220" s="1"/>
       <c r="I220" s="3"/>
       <c r="J220" s="3"/>
       <c r="K220" s="3"/>
@@ -7082,7 +7077,7 @@
       <c r="E221" s="2"/>
       <c r="F221" s="2"/>
       <c r="G221" s="2"/>
-      <c r="H221" s="2"/>
+      <c r="H221" s="1"/>
       <c r="I221" s="3"/>
       <c r="J221" s="3"/>
       <c r="K221" s="3"/>
@@ -7112,7 +7107,7 @@
       <c r="E222" s="2"/>
       <c r="F222" s="2"/>
       <c r="G222" s="2"/>
-      <c r="H222" s="2"/>
+      <c r="H222" s="1"/>
       <c r="I222" s="3"/>
       <c r="J222" s="3"/>
       <c r="K222" s="3"/>
@@ -7142,7 +7137,7 @@
       <c r="E223" s="2"/>
       <c r="F223" s="2"/>
       <c r="G223" s="2"/>
-      <c r="H223" s="2"/>
+      <c r="H223" s="1"/>
       <c r="I223" s="3"/>
       <c r="J223" s="3"/>
       <c r="K223" s="3"/>
@@ -7172,7 +7167,7 @@
       <c r="E224" s="2"/>
       <c r="F224" s="2"/>
       <c r="G224" s="2"/>
-      <c r="H224" s="2"/>
+      <c r="H224" s="1"/>
       <c r="I224" s="3"/>
       <c r="J224" s="3"/>
       <c r="K224" s="3"/>
@@ -7202,7 +7197,7 @@
       <c r="E225" s="2"/>
       <c r="F225" s="2"/>
       <c r="G225" s="2"/>
-      <c r="H225" s="2"/>
+      <c r="H225" s="1"/>
       <c r="I225" s="3"/>
       <c r="J225" s="3"/>
       <c r="K225" s="3"/>
@@ -7232,7 +7227,7 @@
       <c r="E226" s="2"/>
       <c r="F226" s="2"/>
       <c r="G226" s="2"/>
-      <c r="H226" s="2"/>
+      <c r="H226" s="1"/>
       <c r="I226" s="3"/>
       <c r="J226" s="3"/>
       <c r="K226" s="3"/>
@@ -7262,7 +7257,7 @@
       <c r="E227" s="2"/>
       <c r="F227" s="2"/>
       <c r="G227" s="2"/>
-      <c r="H227" s="2"/>
+      <c r="H227" s="1"/>
       <c r="I227" s="3"/>
       <c r="J227" s="3"/>
       <c r="K227" s="3"/>
@@ -7292,7 +7287,7 @@
       <c r="E228" s="2"/>
       <c r="F228" s="2"/>
       <c r="G228" s="2"/>
-      <c r="H228" s="2"/>
+      <c r="H228" s="1"/>
       <c r="I228" s="3"/>
       <c r="J228" s="3"/>
       <c r="K228" s="3"/>
@@ -7322,7 +7317,7 @@
       <c r="E229" s="2"/>
       <c r="F229" s="2"/>
       <c r="G229" s="2"/>
-      <c r="H229" s="2"/>
+      <c r="H229" s="1"/>
       <c r="I229" s="3"/>
       <c r="J229" s="3"/>
       <c r="K229" s="3"/>
@@ -7352,7 +7347,7 @@
       <c r="E230" s="2"/>
       <c r="F230" s="2"/>
       <c r="G230" s="2"/>
-      <c r="H230" s="2"/>
+      <c r="H230" s="1"/>
       <c r="I230" s="3"/>
       <c r="J230" s="3"/>
       <c r="K230" s="3"/>
@@ -7382,7 +7377,7 @@
       <c r="E231" s="2"/>
       <c r="F231" s="2"/>
       <c r="G231" s="2"/>
-      <c r="H231" s="2"/>
+      <c r="H231" s="1"/>
       <c r="I231" s="3"/>
       <c r="J231" s="3"/>
       <c r="K231" s="3"/>
@@ -7412,7 +7407,7 @@
       <c r="E232" s="2"/>
       <c r="F232" s="2"/>
       <c r="G232" s="2"/>
-      <c r="H232" s="2"/>
+      <c r="H232" s="1"/>
       <c r="I232" s="3"/>
       <c r="J232" s="3"/>
       <c r="K232" s="3"/>
@@ -7442,7 +7437,7 @@
       <c r="E233" s="2"/>
       <c r="F233" s="2"/>
       <c r="G233" s="2"/>
-      <c r="H233" s="2"/>
+      <c r="H233" s="1"/>
       <c r="I233" s="3"/>
       <c r="J233" s="3"/>
       <c r="K233" s="3"/>
@@ -7472,7 +7467,7 @@
       <c r="E234" s="2"/>
       <c r="F234" s="2"/>
       <c r="G234" s="2"/>
-      <c r="H234" s="2"/>
+      <c r="H234" s="1"/>
       <c r="I234" s="3"/>
       <c r="J234" s="3"/>
       <c r="K234" s="3"/>
@@ -7502,7 +7497,7 @@
       <c r="E235" s="2"/>
       <c r="F235" s="2"/>
       <c r="G235" s="2"/>
-      <c r="H235" s="2"/>
+      <c r="H235" s="1"/>
       <c r="I235" s="3"/>
       <c r="J235" s="3"/>
       <c r="K235" s="3"/>
@@ -7532,7 +7527,7 @@
       <c r="E236" s="2"/>
       <c r="F236" s="2"/>
       <c r="G236" s="2"/>
-      <c r="H236" s="2"/>
+      <c r="H236" s="1"/>
       <c r="I236" s="3"/>
       <c r="J236" s="3"/>
       <c r="K236" s="3"/>
@@ -7562,7 +7557,7 @@
       <c r="E237" s="2"/>
       <c r="F237" s="2"/>
       <c r="G237" s="2"/>
-      <c r="H237" s="2"/>
+      <c r="H237" s="1"/>
       <c r="I237" s="3"/>
       <c r="J237" s="3"/>
       <c r="K237" s="3"/>
@@ -7592,7 +7587,7 @@
       <c r="E238" s="2"/>
       <c r="F238" s="2"/>
       <c r="G238" s="2"/>
-      <c r="H238" s="2"/>
+      <c r="H238" s="1"/>
       <c r="I238" s="3"/>
       <c r="J238" s="3"/>
       <c r="K238" s="3"/>
@@ -7622,7 +7617,7 @@
       <c r="E239" s="2"/>
       <c r="F239" s="2"/>
       <c r="G239" s="2"/>
-      <c r="H239" s="2"/>
+      <c r="H239" s="1"/>
       <c r="I239" s="3"/>
       <c r="J239" s="3"/>
       <c r="K239" s="3"/>
@@ -7652,7 +7647,7 @@
       <c r="E240" s="2"/>
       <c r="F240" s="2"/>
       <c r="G240" s="2"/>
-      <c r="H240" s="2"/>
+      <c r="H240" s="1"/>
       <c r="I240" s="3"/>
       <c r="J240" s="3"/>
       <c r="K240" s="3"/>
@@ -7682,7 +7677,7 @@
       <c r="E241" s="2"/>
       <c r="F241" s="2"/>
       <c r="G241" s="2"/>
-      <c r="H241" s="2"/>
+      <c r="H241" s="1"/>
       <c r="I241" s="3"/>
       <c r="J241" s="3"/>
       <c r="K241" s="3"/>
@@ -7712,7 +7707,7 @@
       <c r="E242" s="2"/>
       <c r="F242" s="2"/>
       <c r="G242" s="2"/>
-      <c r="H242" s="2"/>
+      <c r="H242" s="1"/>
       <c r="I242" s="3"/>
       <c r="J242" s="3"/>
       <c r="K242" s="3"/>
@@ -7742,7 +7737,7 @@
       <c r="E243" s="2"/>
       <c r="F243" s="2"/>
       <c r="G243" s="2"/>
-      <c r="H243" s="2"/>
+      <c r="H243" s="1"/>
       <c r="I243" s="3"/>
       <c r="J243" s="3"/>
       <c r="K243" s="3"/>
@@ -7772,7 +7767,7 @@
       <c r="E244" s="2"/>
       <c r="F244" s="2"/>
       <c r="G244" s="2"/>
-      <c r="H244" s="2"/>
+      <c r="H244" s="1"/>
       <c r="I244" s="3"/>
       <c r="J244" s="3"/>
       <c r="K244" s="3"/>
@@ -7802,7 +7797,7 @@
       <c r="E245" s="2"/>
       <c r="F245" s="2"/>
       <c r="G245" s="2"/>
-      <c r="H245" s="2"/>
+      <c r="H245" s="1"/>
       <c r="I245" s="3"/>
       <c r="J245" s="3"/>
       <c r="K245" s="3"/>
@@ -7832,7 +7827,7 @@
       <c r="E246" s="2"/>
       <c r="F246" s="2"/>
       <c r="G246" s="2"/>
-      <c r="H246" s="2"/>
+      <c r="H246" s="1"/>
       <c r="I246" s="3"/>
       <c r="J246" s="3"/>
       <c r="K246" s="3"/>
@@ -7862,7 +7857,7 @@
       <c r="E247" s="2"/>
       <c r="F247" s="2"/>
       <c r="G247" s="2"/>
-      <c r="H247" s="2"/>
+      <c r="H247" s="1"/>
       <c r="I247" s="3"/>
       <c r="J247" s="3"/>
       <c r="K247" s="3"/>
@@ -7892,7 +7887,7 @@
       <c r="E248" s="2"/>
       <c r="F248" s="2"/>
       <c r="G248" s="2"/>
-      <c r="H248" s="2"/>
+      <c r="H248" s="1"/>
       <c r="I248" s="3"/>
       <c r="J248" s="3"/>
       <c r="K248" s="3"/>
@@ -7922,7 +7917,7 @@
       <c r="E249" s="2"/>
       <c r="F249" s="2"/>
       <c r="G249" s="2"/>
-      <c r="H249" s="2"/>
+      <c r="H249" s="1"/>
       <c r="I249" s="3"/>
       <c r="J249" s="3"/>
       <c r="K249" s="3"/>
@@ -7952,7 +7947,7 @@
       <c r="E250" s="2"/>
       <c r="F250" s="2"/>
       <c r="G250" s="2"/>
-      <c r="H250" s="2"/>
+      <c r="H250" s="1"/>
       <c r="I250" s="3"/>
       <c r="J250" s="3"/>
       <c r="K250" s="3"/>
@@ -7982,7 +7977,7 @@
       <c r="E251" s="2"/>
       <c r="F251" s="2"/>
       <c r="G251" s="2"/>
-      <c r="H251" s="2"/>
+      <c r="H251" s="1"/>
       <c r="I251" s="3"/>
       <c r="J251" s="3"/>
       <c r="K251" s="3"/>
@@ -8012,7 +8007,7 @@
       <c r="E252" s="2"/>
       <c r="F252" s="2"/>
       <c r="G252" s="2"/>
-      <c r="H252" s="2"/>
+      <c r="H252" s="1"/>
       <c r="I252" s="3"/>
       <c r="J252" s="3"/>
       <c r="K252" s="3"/>
@@ -8042,7 +8037,7 @@
       <c r="E253" s="2"/>
       <c r="F253" s="2"/>
       <c r="G253" s="2"/>
-      <c r="H253" s="2"/>
+      <c r="H253" s="1"/>
       <c r="I253" s="3"/>
       <c r="J253" s="3"/>
       <c r="K253" s="3"/>
@@ -8072,7 +8067,7 @@
       <c r="E254" s="2"/>
       <c r="F254" s="2"/>
       <c r="G254" s="2"/>
-      <c r="H254" s="2"/>
+      <c r="H254" s="1"/>
       <c r="I254" s="3"/>
       <c r="J254" s="3"/>
       <c r="K254" s="3"/>
@@ -8102,7 +8097,7 @@
       <c r="E255" s="2"/>
       <c r="F255" s="2"/>
       <c r="G255" s="2"/>
-      <c r="H255" s="2"/>
+      <c r="H255" s="1"/>
       <c r="I255" s="3"/>
       <c r="J255" s="3"/>
       <c r="K255" s="3"/>
@@ -8132,7 +8127,7 @@
       <c r="E256" s="2"/>
       <c r="F256" s="2"/>
       <c r="G256" s="2"/>
-      <c r="H256" s="2"/>
+      <c r="H256" s="1"/>
       <c r="I256" s="3"/>
       <c r="J256" s="3"/>
       <c r="K256" s="3"/>
@@ -8162,7 +8157,7 @@
       <c r="E257" s="2"/>
       <c r="F257" s="2"/>
       <c r="G257" s="2"/>
-      <c r="H257" s="2"/>
+      <c r="H257" s="1"/>
       <c r="I257" s="3"/>
       <c r="J257" s="3"/>
       <c r="K257" s="3"/>
@@ -8192,7 +8187,7 @@
       <c r="E258" s="2"/>
       <c r="F258" s="2"/>
       <c r="G258" s="2"/>
-      <c r="H258" s="2"/>
+      <c r="H258" s="1"/>
       <c r="I258" s="3"/>
       <c r="J258" s="3"/>
       <c r="K258" s="3"/>
@@ -8222,7 +8217,7 @@
       <c r="E259" s="2"/>
       <c r="F259" s="2"/>
       <c r="G259" s="2"/>
-      <c r="H259" s="2"/>
+      <c r="H259" s="1"/>
       <c r="I259" s="3"/>
       <c r="J259" s="3"/>
       <c r="K259" s="3"/>
@@ -8252,7 +8247,7 @@
       <c r="E260" s="2"/>
       <c r="F260" s="2"/>
       <c r="G260" s="2"/>
-      <c r="H260" s="2"/>
+      <c r="H260" s="1"/>
       <c r="I260" s="3"/>
       <c r="J260" s="3"/>
       <c r="K260" s="3"/>
@@ -8282,7 +8277,7 @@
       <c r="E261" s="2"/>
       <c r="F261" s="2"/>
       <c r="G261" s="2"/>
-      <c r="H261" s="2"/>
+      <c r="H261" s="1"/>
       <c r="I261" s="3"/>
       <c r="J261" s="3"/>
       <c r="K261" s="3"/>
@@ -8312,7 +8307,7 @@
       <c r="E262" s="2"/>
       <c r="F262" s="2"/>
       <c r="G262" s="2"/>
-      <c r="H262" s="2"/>
+      <c r="H262" s="1"/>
       <c r="I262" s="3"/>
       <c r="J262" s="3"/>
       <c r="K262" s="3"/>
@@ -8342,7 +8337,7 @@
       <c r="E263" s="2"/>
       <c r="F263" s="2"/>
       <c r="G263" s="2"/>
-      <c r="H263" s="2"/>
+      <c r="H263" s="1"/>
       <c r="I263" s="3"/>
       <c r="J263" s="3"/>
       <c r="K263" s="3"/>
@@ -8372,7 +8367,7 @@
       <c r="E264" s="2"/>
       <c r="F264" s="2"/>
       <c r="G264" s="2"/>
-      <c r="H264" s="2"/>
+      <c r="H264" s="1"/>
       <c r="I264" s="3"/>
       <c r="J264" s="3"/>
       <c r="K264" s="3"/>
@@ -8402,7 +8397,7 @@
       <c r="E265" s="2"/>
       <c r="F265" s="2"/>
       <c r="G265" s="2"/>
-      <c r="H265" s="2"/>
+      <c r="H265" s="1"/>
       <c r="I265" s="3"/>
       <c r="J265" s="3"/>
       <c r="K265" s="3"/>
@@ -8432,7 +8427,7 @@
       <c r="E266" s="2"/>
       <c r="F266" s="2"/>
       <c r="G266" s="2"/>
-      <c r="H266" s="2"/>
+      <c r="H266" s="1"/>
       <c r="I266" s="3"/>
       <c r="J266" s="3"/>
       <c r="K266" s="3"/>
@@ -8462,7 +8457,7 @@
       <c r="E267" s="2"/>
       <c r="F267" s="2"/>
       <c r="G267" s="2"/>
-      <c r="H267" s="2"/>
+      <c r="H267" s="1"/>
       <c r="I267" s="3"/>
       <c r="J267" s="3"/>
       <c r="K267" s="3"/>
@@ -8492,7 +8487,7 @@
       <c r="E268" s="2"/>
       <c r="F268" s="2"/>
       <c r="G268" s="2"/>
-      <c r="H268" s="2"/>
+      <c r="H268" s="1"/>
       <c r="I268" s="3"/>
       <c r="J268" s="3"/>
       <c r="K268" s="3"/>
@@ -8522,7 +8517,7 @@
       <c r="E269" s="2"/>
       <c r="F269" s="2"/>
       <c r="G269" s="2"/>
-      <c r="H269" s="2"/>
+      <c r="H269" s="1"/>
       <c r="I269" s="3"/>
       <c r="J269" s="3"/>
       <c r="K269" s="3"/>
@@ -8552,7 +8547,7 @@
       <c r="E270" s="2"/>
       <c r="F270" s="2"/>
       <c r="G270" s="2"/>
-      <c r="H270" s="2"/>
+      <c r="H270" s="1"/>
       <c r="I270" s="3"/>
       <c r="J270" s="3"/>
       <c r="K270" s="3"/>
@@ -8582,7 +8577,7 @@
       <c r="E271" s="2"/>
       <c r="F271" s="2"/>
       <c r="G271" s="2"/>
-      <c r="H271" s="2"/>
+      <c r="H271" s="1"/>
       <c r="I271" s="3"/>
       <c r="J271" s="3"/>
       <c r="K271" s="3"/>
@@ -8612,7 +8607,7 @@
       <c r="E272" s="2"/>
       <c r="F272" s="2"/>
       <c r="G272" s="2"/>
-      <c r="H272" s="2"/>
+      <c r="H272" s="1"/>
       <c r="I272" s="3"/>
       <c r="J272" s="3"/>
       <c r="K272" s="3"/>
@@ -8642,7 +8637,7 @@
       <c r="E273" s="2"/>
       <c r="F273" s="2"/>
       <c r="G273" s="2"/>
-      <c r="H273" s="2"/>
+      <c r="H273" s="1"/>
       <c r="I273" s="3"/>
       <c r="J273" s="3"/>
       <c r="K273" s="3"/>
@@ -8672,7 +8667,7 @@
       <c r="E274" s="2"/>
       <c r="F274" s="2"/>
       <c r="G274" s="2"/>
-      <c r="H274" s="2"/>
+      <c r="H274" s="1"/>
       <c r="I274" s="3"/>
       <c r="J274" s="3"/>
       <c r="K274" s="3"/>
@@ -8702,7 +8697,7 @@
       <c r="E275" s="2"/>
       <c r="F275" s="2"/>
       <c r="G275" s="2"/>
-      <c r="H275" s="2"/>
+      <c r="H275" s="1"/>
       <c r="I275" s="3"/>
       <c r="J275" s="3"/>
       <c r="K275" s="3"/>
@@ -8732,7 +8727,7 @@
       <c r="E276" s="2"/>
       <c r="F276" s="2"/>
       <c r="G276" s="2"/>
-      <c r="H276" s="2"/>
+      <c r="H276" s="1"/>
       <c r="I276" s="3"/>
       <c r="J276" s="3"/>
       <c r="K276" s="3"/>
@@ -8762,7 +8757,7 @@
       <c r="E277" s="2"/>
       <c r="F277" s="2"/>
       <c r="G277" s="2"/>
-      <c r="H277" s="2"/>
+      <c r="H277" s="1"/>
       <c r="I277" s="3"/>
       <c r="J277" s="3"/>
       <c r="K277" s="3"/>
@@ -8792,7 +8787,7 @@
       <c r="E278" s="2"/>
       <c r="F278" s="2"/>
       <c r="G278" s="2"/>
-      <c r="H278" s="2"/>
+      <c r="H278" s="1"/>
       <c r="I278" s="3"/>
       <c r="J278" s="3"/>
       <c r="K278" s="3"/>
@@ -8822,7 +8817,7 @@
       <c r="E279" s="2"/>
       <c r="F279" s="2"/>
       <c r="G279" s="2"/>
-      <c r="H279" s="2"/>
+      <c r="H279" s="1"/>
       <c r="I279" s="3"/>
       <c r="J279" s="3"/>
       <c r="K279" s="3"/>
@@ -8852,7 +8847,7 @@
       <c r="E280" s="2"/>
       <c r="F280" s="2"/>
       <c r="G280" s="2"/>
-      <c r="H280" s="2"/>
+      <c r="H280" s="1"/>
       <c r="I280" s="3"/>
       <c r="J280" s="3"/>
       <c r="K280" s="3"/>
@@ -8882,7 +8877,7 @@
       <c r="E281" s="2"/>
       <c r="F281" s="2"/>
       <c r="G281" s="2"/>
-      <c r="H281" s="2"/>
+      <c r="H281" s="1"/>
       <c r="I281" s="3"/>
       <c r="J281" s="3"/>
       <c r="K281" s="3"/>
@@ -8912,7 +8907,7 @@
       <c r="E282" s="2"/>
       <c r="F282" s="2"/>
       <c r="G282" s="2"/>
-      <c r="H282" s="2"/>
+      <c r="H282" s="1"/>
       <c r="I282" s="3"/>
       <c r="J282" s="3"/>
       <c r="K282" s="3"/>
@@ -8942,7 +8937,7 @@
       <c r="E283" s="2"/>
       <c r="F283" s="2"/>
       <c r="G283" s="2"/>
-      <c r="H283" s="2"/>
+      <c r="H283" s="1"/>
       <c r="I283" s="3"/>
       <c r="J283" s="3"/>
       <c r="K283" s="3"/>
@@ -8972,7 +8967,7 @@
       <c r="E284" s="2"/>
       <c r="F284" s="2"/>
       <c r="G284" s="2"/>
-      <c r="H284" s="2"/>
+      <c r="H284" s="1"/>
       <c r="I284" s="3"/>
       <c r="J284" s="3"/>
       <c r="K284" s="3"/>
@@ -9002,7 +8997,7 @@
       <c r="E285" s="2"/>
       <c r="F285" s="2"/>
       <c r="G285" s="2"/>
-      <c r="H285" s="2"/>
+      <c r="H285" s="1"/>
       <c r="I285" s="3"/>
       <c r="J285" s="3"/>
       <c r="K285" s="3"/>
@@ -9032,7 +9027,7 @@
       <c r="E286" s="2"/>
       <c r="F286" s="2"/>
       <c r="G286" s="2"/>
-      <c r="H286" s="2"/>
+      <c r="H286" s="1"/>
       <c r="I286" s="3"/>
       <c r="J286" s="3"/>
       <c r="K286" s="3"/>
@@ -9062,7 +9057,7 @@
       <c r="E287" s="2"/>
       <c r="F287" s="2"/>
       <c r="G287" s="2"/>
-      <c r="H287" s="2"/>
+      <c r="H287" s="1"/>
       <c r="I287" s="3"/>
       <c r="J287" s="3"/>
       <c r="K287" s="3"/>
@@ -9092,7 +9087,7 @@
       <c r="E288" s="2"/>
       <c r="F288" s="2"/>
       <c r="G288" s="2"/>
-      <c r="H288" s="2"/>
+      <c r="H288" s="1"/>
       <c r="I288" s="3"/>
       <c r="J288" s="3"/>
       <c r="K288" s="3"/>
@@ -9122,7 +9117,7 @@
       <c r="E289" s="2"/>
       <c r="F289" s="2"/>
       <c r="G289" s="2"/>
-      <c r="H289" s="2"/>
+      <c r="H289" s="1"/>
       <c r="I289" s="3"/>
       <c r="J289" s="3"/>
       <c r="K289" s="3"/>
@@ -9152,7 +9147,7 @@
       <c r="E290" s="2"/>
       <c r="F290" s="2"/>
       <c r="G290" s="2"/>
-      <c r="H290" s="2"/>
+      <c r="H290" s="1"/>
       <c r="I290" s="3"/>
       <c r="J290" s="3"/>
       <c r="K290" s="3"/>
@@ -9182,7 +9177,7 @@
       <c r="E291" s="2"/>
       <c r="F291" s="2"/>
       <c r="G291" s="2"/>
-      <c r="H291" s="2"/>
+      <c r="H291" s="1"/>
       <c r="I291" s="3"/>
       <c r="J291" s="3"/>
       <c r="K291" s="3"/>
@@ -9212,7 +9207,7 @@
       <c r="E292" s="2"/>
       <c r="F292" s="2"/>
       <c r="G292" s="2"/>
-      <c r="H292" s="2"/>
+      <c r="H292" s="1"/>
       <c r="I292" s="3"/>
       <c r="J292" s="3"/>
       <c r="K292" s="3"/>
@@ -9242,7 +9237,7 @@
       <c r="E293" s="2"/>
       <c r="F293" s="2"/>
       <c r="G293" s="2"/>
-      <c r="H293" s="2"/>
+      <c r="H293" s="1"/>
       <c r="I293" s="3"/>
       <c r="J293" s="3"/>
       <c r="K293" s="3"/>
@@ -9272,7 +9267,7 @@
       <c r="E294" s="2"/>
       <c r="F294" s="2"/>
       <c r="G294" s="2"/>
-      <c r="H294" s="2"/>
+      <c r="H294" s="1"/>
       <c r="I294" s="3"/>
       <c r="J294" s="3"/>
       <c r="K294" s="3"/>
@@ -9302,7 +9297,7 @@
       <c r="E295" s="2"/>
       <c r="F295" s="2"/>
       <c r="G295" s="2"/>
-      <c r="H295" s="2"/>
+      <c r="H295" s="1"/>
       <c r="I295" s="3"/>
       <c r="J295" s="3"/>
       <c r="K295" s="3"/>
@@ -9332,7 +9327,7 @@
       <c r="E296" s="2"/>
       <c r="F296" s="2"/>
       <c r="G296" s="2"/>
-      <c r="H296" s="2"/>
+      <c r="H296" s="1"/>
       <c r="I296" s="3"/>
       <c r="J296" s="3"/>
       <c r="K296" s="3"/>
@@ -9362,7 +9357,7 @@
       <c r="E297" s="2"/>
       <c r="F297" s="2"/>
       <c r="G297" s="2"/>
-      <c r="H297" s="2"/>
+      <c r="H297" s="1"/>
       <c r="I297" s="3"/>
       <c r="J297" s="3"/>
       <c r="K297" s="3"/>
@@ -9392,7 +9387,7 @@
       <c r="E298" s="2"/>
       <c r="F298" s="2"/>
       <c r="G298" s="2"/>
-      <c r="H298" s="2"/>
+      <c r="H298" s="1"/>
       <c r="I298" s="3"/>
       <c r="J298" s="3"/>
       <c r="K298" s="3"/>
@@ -9422,7 +9417,7 @@
       <c r="E299" s="2"/>
       <c r="F299" s="2"/>
       <c r="G299" s="2"/>
-      <c r="H299" s="2"/>
+      <c r="H299" s="1"/>
       <c r="I299" s="3"/>
       <c r="J299" s="3"/>
       <c r="K299" s="3"/>
@@ -9452,7 +9447,7 @@
       <c r="E300" s="2"/>
       <c r="F300" s="2"/>
       <c r="G300" s="2"/>
-      <c r="H300" s="2"/>
+      <c r="H300" s="1"/>
       <c r="I300" s="3"/>
       <c r="J300" s="3"/>
       <c r="K300" s="3"/>
@@ -9482,7 +9477,7 @@
       <c r="E301" s="2"/>
       <c r="F301" s="2"/>
       <c r="G301" s="2"/>
-      <c r="H301" s="2"/>
+      <c r="H301" s="1"/>
       <c r="I301" s="3"/>
       <c r="J301" s="3"/>
       <c r="K301" s="3"/>
@@ -9512,7 +9507,7 @@
       <c r="E302" s="2"/>
       <c r="F302" s="2"/>
       <c r="G302" s="2"/>
-      <c r="H302" s="2"/>
+      <c r="H302" s="1"/>
       <c r="I302" s="3"/>
       <c r="J302" s="3"/>
       <c r="K302" s="3"/>
@@ -9542,7 +9537,7 @@
       <c r="E303" s="2"/>
       <c r="F303" s="2"/>
       <c r="G303" s="2"/>
-      <c r="H303" s="2"/>
+      <c r="H303" s="1"/>
       <c r="I303" s="3"/>
       <c r="J303" s="3"/>
       <c r="K303" s="3"/>
@@ -9572,7 +9567,7 @@
       <c r="E304" s="2"/>
       <c r="F304" s="2"/>
       <c r="G304" s="2"/>
-      <c r="H304" s="2"/>
+      <c r="H304" s="1"/>
       <c r="I304" s="3"/>
       <c r="J304" s="3"/>
       <c r="K304" s="3"/>
@@ -9602,7 +9597,7 @@
       <c r="E305" s="2"/>
       <c r="F305" s="2"/>
       <c r="G305" s="2"/>
-      <c r="H305" s="2"/>
+      <c r="H305" s="1"/>
       <c r="I305" s="3"/>
       <c r="J305" s="3"/>
       <c r="K305" s="3"/>
@@ -9632,7 +9627,7 @@
       <c r="E306" s="2"/>
       <c r="F306" s="2"/>
       <c r="G306" s="2"/>
-      <c r="H306" s="2"/>
+      <c r="H306" s="1"/>
       <c r="I306" s="3"/>
       <c r="J306" s="3"/>
       <c r="K306" s="3"/>
@@ -9662,7 +9657,7 @@
       <c r="E307" s="2"/>
       <c r="F307" s="2"/>
       <c r="G307" s="2"/>
-      <c r="H307" s="2"/>
+      <c r="H307" s="1"/>
       <c r="I307" s="3"/>
       <c r="J307" s="3"/>
       <c r="K307" s="3"/>
@@ -9692,7 +9687,7 @@
       <c r="E308" s="2"/>
       <c r="F308" s="2"/>
       <c r="G308" s="2"/>
-      <c r="H308" s="2"/>
+      <c r="H308" s="1"/>
       <c r="I308" s="3"/>
       <c r="J308" s="3"/>
       <c r="K308" s="3"/>
@@ -9722,7 +9717,7 @@
       <c r="E309" s="2"/>
       <c r="F309" s="2"/>
       <c r="G309" s="2"/>
-      <c r="H309" s="2"/>
+      <c r="H309" s="1"/>
       <c r="I309" s="3"/>
       <c r="J309" s="3"/>
       <c r="K309" s="3"/>
@@ -9752,7 +9747,7 @@
       <c r="E310" s="2"/>
       <c r="F310" s="2"/>
       <c r="G310" s="2"/>
-      <c r="H310" s="2"/>
+      <c r="H310" s="1"/>
       <c r="I310" s="3"/>
       <c r="J310" s="3"/>
       <c r="K310" s="3"/>
@@ -9782,7 +9777,7 @@
       <c r="E311" s="2"/>
       <c r="F311" s="2"/>
       <c r="G311" s="2"/>
-      <c r="H311" s="2"/>
+      <c r="H311" s="1"/>
       <c r="I311" s="3"/>
       <c r="J311" s="3"/>
       <c r="K311" s="3"/>
@@ -9812,7 +9807,7 @@
       <c r="E312" s="2"/>
       <c r="F312" s="2"/>
       <c r="G312" s="2"/>
-      <c r="H312" s="2"/>
+      <c r="H312" s="1"/>
       <c r="I312" s="3"/>
       <c r="J312" s="3"/>
       <c r="K312" s="3"/>
@@ -9842,7 +9837,7 @@
       <c r="E313" s="2"/>
       <c r="F313" s="2"/>
       <c r="G313" s="2"/>
-      <c r="H313" s="2"/>
+      <c r="H313" s="1"/>
       <c r="I313" s="3"/>
       <c r="J313" s="3"/>
       <c r="K313" s="3"/>
@@ -9872,7 +9867,7 @@
       <c r="E314" s="2"/>
       <c r="F314" s="2"/>
       <c r="G314" s="2"/>
-      <c r="H314" s="2"/>
+      <c r="H314" s="1"/>
       <c r="I314" s="3"/>
       <c r="J314" s="3"/>
       <c r="K314" s="3"/>
@@ -9902,7 +9897,7 @@
       <c r="E315" s="2"/>
       <c r="F315" s="2"/>
       <c r="G315" s="2"/>
-      <c r="H315" s="2"/>
+      <c r="H315" s="1"/>
       <c r="I315" s="3"/>
       <c r="J315" s="3"/>
       <c r="K315" s="3"/>
@@ -9932,7 +9927,7 @@
       <c r="E316" s="2"/>
       <c r="F316" s="2"/>
       <c r="G316" s="2"/>
-      <c r="H316" s="2"/>
+      <c r="H316" s="1"/>
       <c r="I316" s="3"/>
       <c r="J316" s="3"/>
       <c r="K316" s="3"/>
@@ -9962,7 +9957,7 @@
       <c r="E317" s="2"/>
       <c r="F317" s="2"/>
       <c r="G317" s="2"/>
-      <c r="H317" s="2"/>
+      <c r="H317" s="1"/>
       <c r="I317" s="3"/>
       <c r="J317" s="3"/>
       <c r="K317" s="3"/>
@@ -9992,7 +9987,7 @@
       <c r="E318" s="2"/>
       <c r="F318" s="2"/>
       <c r="G318" s="2"/>
-      <c r="H318" s="2"/>
+      <c r="H318" s="1"/>
       <c r="I318" s="3"/>
       <c r="J318" s="3"/>
       <c r="K318" s="3"/>
@@ -10022,7 +10017,7 @@
       <c r="E319" s="2"/>
       <c r="F319" s="2"/>
       <c r="G319" s="2"/>
-      <c r="H319" s="2"/>
+      <c r="H319" s="1"/>
       <c r="I319" s="3"/>
       <c r="J319" s="3"/>
       <c r="K319" s="3"/>
@@ -10052,7 +10047,7 @@
       <c r="E320" s="2"/>
       <c r="F320" s="2"/>
       <c r="G320" s="2"/>
-      <c r="H320" s="2"/>
+      <c r="H320" s="1"/>
       <c r="I320" s="3"/>
       <c r="J320" s="3"/>
       <c r="K320" s="3"/>
@@ -10082,7 +10077,7 @@
       <c r="E321" s="2"/>
       <c r="F321" s="2"/>
       <c r="G321" s="2"/>
-      <c r="H321" s="2"/>
+      <c r="H321" s="1"/>
       <c r="I321" s="3"/>
       <c r="J321" s="3"/>
       <c r="K321" s="3"/>
@@ -10112,7 +10107,7 @@
       <c r="E322" s="2"/>
       <c r="F322" s="2"/>
       <c r="G322" s="2"/>
-      <c r="H322" s="2"/>
+      <c r="H322" s="1"/>
       <c r="I322" s="3"/>
       <c r="J322" s="3"/>
       <c r="K322" s="3"/>
@@ -10142,7 +10137,7 @@
       <c r="E323" s="2"/>
       <c r="F323" s="2"/>
       <c r="G323" s="2"/>
-      <c r="H323" s="2"/>
+      <c r="H323" s="1"/>
       <c r="I323" s="3"/>
       <c r="J323" s="3"/>
       <c r="K323" s="3"/>
@@ -10172,7 +10167,7 @@
       <c r="E324" s="2"/>
       <c r="F324" s="2"/>
       <c r="G324" s="2"/>
-      <c r="H324" s="2"/>
+      <c r="H324" s="1"/>
       <c r="I324" s="3"/>
       <c r="J324" s="3"/>
       <c r="K324" s="3"/>
@@ -10202,7 +10197,7 @@
       <c r="E325" s="2"/>
       <c r="F325" s="2"/>
       <c r="G325" s="2"/>
-      <c r="H325" s="2"/>
+      <c r="H325" s="1"/>
       <c r="I325" s="3"/>
       <c r="J325" s="3"/>
       <c r="K325" s="3"/>
@@ -10232,7 +10227,7 @@
       <c r="E326" s="2"/>
       <c r="F326" s="2"/>
       <c r="G326" s="2"/>
-      <c r="H326" s="2"/>
+      <c r="H326" s="1"/>
       <c r="I326" s="3"/>
       <c r="J326" s="3"/>
       <c r="K326" s="3"/>
@@ -10262,7 +10257,7 @@
       <c r="E327" s="2"/>
       <c r="F327" s="2"/>
       <c r="G327" s="2"/>
-      <c r="H327" s="2"/>
+      <c r="H327" s="1"/>
       <c r="I327" s="3"/>
       <c r="J327" s="3"/>
       <c r="K327" s="3"/>
@@ -10292,7 +10287,7 @@
       <c r="E328" s="2"/>
       <c r="F328" s="2"/>
       <c r="G328" s="2"/>
-      <c r="H328" s="2"/>
+      <c r="H328" s="1"/>
       <c r="I328" s="3"/>
       <c r="J328" s="3"/>
       <c r="K328" s="3"/>
@@ -10322,7 +10317,7 @@
       <c r="E329" s="2"/>
       <c r="F329" s="2"/>
       <c r="G329" s="2"/>
-      <c r="H329" s="2"/>
+      <c r="H329" s="1"/>
       <c r="I329" s="3"/>
       <c r="J329" s="3"/>
       <c r="K329" s="3"/>
@@ -10352,7 +10347,7 @@
       <c r="E330" s="2"/>
       <c r="F330" s="2"/>
       <c r="G330" s="2"/>
-      <c r="H330" s="2"/>
+      <c r="H330" s="1"/>
       <c r="I330" s="3"/>
       <c r="J330" s="3"/>
       <c r="K330" s="3"/>
@@ -10382,7 +10377,7 @@
       <c r="E331" s="2"/>
       <c r="F331" s="2"/>
       <c r="G331" s="2"/>
-      <c r="H331" s="2"/>
+      <c r="H331" s="1"/>
       <c r="I331" s="3"/>
       <c r="J331" s="3"/>
       <c r="K331" s="3"/>
@@ -10412,7 +10407,7 @@
       <c r="E332" s="2"/>
       <c r="F332" s="2"/>
       <c r="G332" s="2"/>
-      <c r="H332" s="2"/>
+      <c r="H332" s="1"/>
       <c r="I332" s="3"/>
       <c r="J332" s="3"/>
       <c r="K332" s="3"/>
@@ -10442,7 +10437,7 @@
       <c r="E333" s="2"/>
       <c r="F333" s="2"/>
       <c r="G333" s="2"/>
-      <c r="H333" s="2"/>
+      <c r="H333" s="1"/>
       <c r="I333" s="3"/>
       <c r="J333" s="3"/>
       <c r="K333" s="3"/>
@@ -10472,7 +10467,7 @@
       <c r="E334" s="2"/>
       <c r="F334" s="2"/>
       <c r="G334" s="2"/>
-      <c r="H334" s="2"/>
+      <c r="H334" s="1"/>
       <c r="I334" s="3"/>
       <c r="J334" s="3"/>
       <c r="K334" s="3"/>
@@ -10502,7 +10497,7 @@
       <c r="E335" s="2"/>
       <c r="F335" s="2"/>
       <c r="G335" s="2"/>
-      <c r="H335" s="2"/>
+      <c r="H335" s="1"/>
       <c r="I335" s="3"/>
       <c r="J335" s="3"/>
       <c r="K335" s="3"/>
@@ -10532,7 +10527,7 @@
       <c r="E336" s="2"/>
       <c r="F336" s="2"/>
       <c r="G336" s="2"/>
-      <c r="H336" s="2"/>
+      <c r="H336" s="1"/>
       <c r="I336" s="3"/>
       <c r="J336" s="3"/>
       <c r="K336" s="3"/>
@@ -10562,7 +10557,7 @@
       <c r="E337" s="2"/>
       <c r="F337" s="2"/>
       <c r="G337" s="2"/>
-      <c r="H337" s="2"/>
+      <c r="H337" s="1"/>
       <c r="I337" s="3"/>
       <c r="J337" s="3"/>
       <c r="K337" s="3"/>
@@ -10592,7 +10587,7 @@
       <c r="E338" s="2"/>
       <c r="F338" s="2"/>
       <c r="G338" s="2"/>
-      <c r="H338" s="2"/>
+      <c r="H338" s="1"/>
       <c r="I338" s="3"/>
       <c r="J338" s="3"/>
       <c r="K338" s="3"/>
@@ -10622,7 +10617,7 @@
       <c r="E339" s="2"/>
       <c r="F339" s="2"/>
       <c r="G339" s="2"/>
-      <c r="H339" s="2"/>
+      <c r="H339" s="1"/>
       <c r="I339" s="3"/>
       <c r="J339" s="3"/>
       <c r="K339" s="3"/>
@@ -10652,7 +10647,7 @@
       <c r="E340" s="2"/>
       <c r="F340" s="2"/>
       <c r="G340" s="2"/>
-      <c r="H340" s="2"/>
+      <c r="H340" s="1"/>
       <c r="I340" s="3"/>
       <c r="J340" s="3"/>
       <c r="K340" s="3"/>
@@ -10682,7 +10677,7 @@
       <c r="E341" s="2"/>
       <c r="F341" s="2"/>
       <c r="G341" s="2"/>
-      <c r="H341" s="2"/>
+      <c r="H341" s="1"/>
       <c r="I341" s="3"/>
       <c r="J341" s="3"/>
       <c r="K341" s="3"/>
@@ -10712,7 +10707,7 @@
       <c r="E342" s="2"/>
       <c r="F342" s="2"/>
       <c r="G342" s="2"/>
-      <c r="H342" s="2"/>
+      <c r="H342" s="1"/>
       <c r="I342" s="3"/>
       <c r="J342" s="3"/>
       <c r="K342" s="3"/>
@@ -10742,7 +10737,7 @@
       <c r="E343" s="2"/>
       <c r="F343" s="2"/>
       <c r="G343" s="2"/>
-      <c r="H343" s="2"/>
+      <c r="H343" s="1"/>
       <c r="I343" s="3"/>
       <c r="J343" s="3"/>
       <c r="K343" s="3"/>
@@ -10772,7 +10767,7 @@
       <c r="E344" s="2"/>
       <c r="F344" s="2"/>
       <c r="G344" s="2"/>
-      <c r="H344" s="2"/>
+      <c r="H344" s="1"/>
       <c r="I344" s="3"/>
       <c r="J344" s="3"/>
       <c r="K344" s="3"/>
@@ -10802,7 +10797,7 @@
       <c r="E345" s="2"/>
       <c r="F345" s="2"/>
       <c r="G345" s="2"/>
-      <c r="H345" s="2"/>
+      <c r="H345" s="1"/>
       <c r="I345" s="3"/>
       <c r="J345" s="3"/>
       <c r="K345" s="3"/>
@@ -10832,7 +10827,7 @@
       <c r="E346" s="2"/>
       <c r="F346" s="2"/>
       <c r="G346" s="2"/>
-      <c r="H346" s="2"/>
+      <c r="H346" s="1"/>
       <c r="I346" s="3"/>
       <c r="J346" s="3"/>
       <c r="K346" s="3"/>
@@ -10862,7 +10857,7 @@
       <c r="E347" s="2"/>
       <c r="F347" s="2"/>
       <c r="G347" s="2"/>
-      <c r="H347" s="2"/>
+      <c r="H347" s="1"/>
       <c r="I347" s="3"/>
       <c r="J347" s="3"/>
       <c r="K347" s="3"/>
@@ -10892,7 +10887,7 @@
       <c r="E348" s="2"/>
       <c r="F348" s="2"/>
       <c r="G348" s="2"/>
-      <c r="H348" s="2"/>
+      <c r="H348" s="1"/>
       <c r="I348" s="3"/>
       <c r="J348" s="3"/>
       <c r="K348" s="3"/>
@@ -10922,7 +10917,7 @@
       <c r="E349" s="2"/>
       <c r="F349" s="2"/>
       <c r="G349" s="2"/>
-      <c r="H349" s="2"/>
+      <c r="H349" s="1"/>
       <c r="I349" s="3"/>
       <c r="J349" s="3"/>
       <c r="K349" s="3"/>
@@ -10952,7 +10947,7 @@
       <c r="E350" s="2"/>
       <c r="F350" s="2"/>
       <c r="G350" s="2"/>
-      <c r="H350" s="2"/>
+      <c r="H350" s="1"/>
       <c r="I350" s="3"/>
       <c r="J350" s="3"/>
       <c r="K350" s="3"/>
@@ -10982,7 +10977,7 @@
       <c r="E351" s="2"/>
       <c r="F351" s="2"/>
       <c r="G351" s="2"/>
-      <c r="H351" s="2"/>
+      <c r="H351" s="1"/>
       <c r="I351" s="3"/>
       <c r="J351" s="3"/>
       <c r="K351" s="3"/>
@@ -11012,7 +11007,7 @@
       <c r="E352" s="2"/>
       <c r="F352" s="2"/>
       <c r="G352" s="2"/>
-      <c r="H352" s="2"/>
+      <c r="H352" s="1"/>
       <c r="I352" s="3"/>
       <c r="J352" s="3"/>
       <c r="K352" s="3"/>
@@ -11042,7 +11037,7 @@
       <c r="E353" s="2"/>
       <c r="F353" s="2"/>
       <c r="G353" s="2"/>
-      <c r="H353" s="2"/>
+      <c r="H353" s="1"/>
       <c r="I353" s="3"/>
       <c r="J353" s="3"/>
       <c r="K353" s="3"/>
@@ -11072,7 +11067,7 @@
       <c r="E354" s="2"/>
       <c r="F354" s="2"/>
       <c r="G354" s="2"/>
-      <c r="H354" s="2"/>
+      <c r="H354" s="1"/>
       <c r="I354" s="3"/>
       <c r="J354" s="3"/>
       <c r="K354" s="3"/>
@@ -11102,7 +11097,7 @@
       <c r="E355" s="2"/>
       <c r="F355" s="2"/>
       <c r="G355" s="2"/>
-      <c r="H355" s="2"/>
+      <c r="H355" s="1"/>
       <c r="I355" s="3"/>
       <c r="J355" s="3"/>
       <c r="K355" s="3"/>
@@ -11132,7 +11127,7 @@
       <c r="E356" s="2"/>
       <c r="F356" s="2"/>
       <c r="G356" s="2"/>
-      <c r="H356" s="2"/>
+      <c r="H356" s="1"/>
       <c r="I356" s="3"/>
       <c r="J356" s="3"/>
       <c r="K356" s="3"/>
@@ -11162,7 +11157,7 @@
       <c r="E357" s="2"/>
       <c r="F357" s="2"/>
       <c r="G357" s="2"/>
-      <c r="H357" s="2"/>
+      <c r="H357" s="1"/>
       <c r="I357" s="3"/>
       <c r="J357" s="3"/>
       <c r="K357" s="3"/>
@@ -11192,7 +11187,7 @@
       <c r="E358" s="2"/>
       <c r="F358" s="2"/>
       <c r="G358" s="2"/>
-      <c r="H358" s="2"/>
+      <c r="H358" s="1"/>
       <c r="I358" s="3"/>
       <c r="J358" s="3"/>
       <c r="K358" s="3"/>
@@ -11222,7 +11217,7 @@
       <c r="E359" s="2"/>
       <c r="F359" s="2"/>
       <c r="G359" s="2"/>
-      <c r="H359" s="2"/>
+      <c r="H359" s="1"/>
       <c r="I359" s="3"/>
       <c r="J359" s="3"/>
       <c r="K359" s="3"/>
@@ -11252,7 +11247,7 @@
       <c r="E360" s="2"/>
       <c r="F360" s="2"/>
       <c r="G360" s="2"/>
-      <c r="H360" s="2"/>
+      <c r="H360" s="1"/>
       <c r="I360" s="3"/>
       <c r="J360" s="3"/>
       <c r="K360" s="3"/>
@@ -11282,7 +11277,7 @@
       <c r="E361" s="2"/>
       <c r="F361" s="2"/>
       <c r="G361" s="2"/>
-      <c r="H361" s="2"/>
+      <c r="H361" s="1"/>
       <c r="I361" s="3"/>
       <c r="J361" s="3"/>
       <c r="K361" s="3"/>
@@ -11312,7 +11307,7 @@
       <c r="E362" s="2"/>
       <c r="F362" s="2"/>
       <c r="G362" s="2"/>
-      <c r="H362" s="2"/>
+      <c r="H362" s="1"/>
       <c r="I362" s="3"/>
       <c r="J362" s="3"/>
       <c r="K362" s="3"/>
@@ -11342,7 +11337,7 @@
       <c r="E363" s="2"/>
       <c r="F363" s="2"/>
       <c r="G363" s="2"/>
-      <c r="H363" s="2"/>
+      <c r="H363" s="1"/>
       <c r="I363" s="3"/>
       <c r="J363" s="3"/>
       <c r="K363" s="3"/>
@@ -11372,7 +11367,7 @@
       <c r="E364" s="2"/>
       <c r="F364" s="2"/>
       <c r="G364" s="2"/>
-      <c r="H364" s="2"/>
+      <c r="H364" s="1"/>
       <c r="I364" s="3"/>
       <c r="J364" s="3"/>
       <c r="K364" s="3"/>
@@ -11402,7 +11397,7 @@
       <c r="E365" s="2"/>
       <c r="F365" s="2"/>
       <c r="G365" s="2"/>
-      <c r="H365" s="2"/>
+      <c r="H365" s="1"/>
       <c r="I365" s="3"/>
       <c r="J365" s="3"/>
       <c r="K365" s="3"/>
@@ -11432,7 +11427,7 @@
       <c r="E366" s="2"/>
       <c r="F366" s="2"/>
       <c r="G366" s="2"/>
-      <c r="H366" s="2"/>
+      <c r="H366" s="1"/>
       <c r="I366" s="3"/>
       <c r="J366" s="3"/>
       <c r="K366" s="3"/>
@@ -11462,7 +11457,7 @@
       <c r="E367" s="2"/>
       <c r="F367" s="2"/>
       <c r="G367" s="2"/>
-      <c r="H367" s="2"/>
+      <c r="H367" s="1"/>
       <c r="I367" s="3"/>
       <c r="J367" s="3"/>
       <c r="K367" s="3"/>
@@ -11492,7 +11487,7 @@
       <c r="E368" s="2"/>
       <c r="F368" s="2"/>
       <c r="G368" s="2"/>
-      <c r="H368" s="2"/>
+      <c r="H368" s="1"/>
       <c r="I368" s="3"/>
       <c r="J368" s="3"/>
       <c r="K368" s="3"/>
@@ -11522,7 +11517,7 @@
       <c r="E369" s="2"/>
       <c r="F369" s="2"/>
       <c r="G369" s="2"/>
-      <c r="H369" s="2"/>
+      <c r="H369" s="1"/>
       <c r="I369" s="3"/>
       <c r="J369" s="3"/>
       <c r="K369" s="3"/>
@@ -11552,7 +11547,7 @@
       <c r="E370" s="2"/>
       <c r="F370" s="2"/>
       <c r="G370" s="2"/>
-      <c r="H370" s="2"/>
+      <c r="H370" s="1"/>
       <c r="I370" s="3"/>
       <c r="J370" s="3"/>
       <c r="K370" s="3"/>
@@ -11582,7 +11577,7 @@
       <c r="E371" s="2"/>
       <c r="F371" s="2"/>
       <c r="G371" s="2"/>
-      <c r="H371" s="2"/>
+      <c r="H371" s="1"/>
       <c r="I371" s="3"/>
       <c r="J371" s="3"/>
       <c r="K371" s="3"/>
@@ -11612,7 +11607,7 @@
       <c r="E372" s="2"/>
       <c r="F372" s="2"/>
       <c r="G372" s="2"/>
-      <c r="H372" s="2"/>
+      <c r="H372" s="1"/>
       <c r="I372" s="3"/>
       <c r="J372" s="3"/>
       <c r="K372" s="3"/>
@@ -11642,7 +11637,7 @@
       <c r="E373" s="2"/>
       <c r="F373" s="2"/>
       <c r="G373" s="2"/>
-      <c r="H373" s="2"/>
+      <c r="H373" s="1"/>
       <c r="I373" s="3"/>
       <c r="J373" s="3"/>
       <c r="K373" s="3"/>
@@ -11672,7 +11667,7 @@
       <c r="E374" s="2"/>
       <c r="F374" s="2"/>
       <c r="G374" s="2"/>
-      <c r="H374" s="2"/>
+      <c r="H374" s="1"/>
       <c r="I374" s="3"/>
       <c r="J374" s="3"/>
       <c r="K374" s="3"/>
@@ -11702,7 +11697,7 @@
       <c r="E375" s="2"/>
       <c r="F375" s="2"/>
       <c r="G375" s="2"/>
-      <c r="H375" s="2"/>
+      <c r="H375" s="1"/>
       <c r="I375" s="3"/>
       <c r="J375" s="3"/>
       <c r="K375" s="3"/>
@@ -11732,7 +11727,7 @@
       <c r="E376" s="2"/>
       <c r="F376" s="2"/>
       <c r="G376" s="2"/>
-      <c r="H376" s="2"/>
+      <c r="H376" s="1"/>
       <c r="I376" s="3"/>
       <c r="J376" s="3"/>
       <c r="K376" s="3"/>
@@ -11762,7 +11757,7 @@
       <c r="E377" s="2"/>
       <c r="F377" s="2"/>
       <c r="G377" s="2"/>
-      <c r="H377" s="2"/>
+      <c r="H377" s="1"/>
       <c r="I377" s="3"/>
       <c r="J377" s="3"/>
       <c r="K377" s="3"/>
@@ -11792,7 +11787,7 @@
       <c r="E378" s="2"/>
       <c r="F378" s="2"/>
       <c r="G378" s="2"/>
-      <c r="H378" s="2"/>
+      <c r="H378" s="1"/>
       <c r="I378" s="3"/>
       <c r="J378" s="3"/>
       <c r="K378" s="3"/>
@@ -11822,7 +11817,7 @@
       <c r="E379" s="2"/>
       <c r="F379" s="2"/>
       <c r="G379" s="2"/>
-      <c r="H379" s="2"/>
+      <c r="H379" s="1"/>
       <c r="I379" s="3"/>
       <c r="J379" s="3"/>
       <c r="K379" s="3"/>
@@ -11852,7 +11847,7 @@
       <c r="E380" s="2"/>
       <c r="F380" s="2"/>
       <c r="G380" s="2"/>
-      <c r="H380" s="2"/>
+      <c r="H380" s="1"/>
       <c r="I380" s="3"/>
       <c r="J380" s="3"/>
       <c r="K380" s="3"/>
@@ -11882,7 +11877,7 @@
       <c r="E381" s="2"/>
       <c r="F381" s="2"/>
       <c r="G381" s="2"/>
-      <c r="H381" s="2"/>
+      <c r="H381" s="1"/>
       <c r="I381" s="3"/>
       <c r="J381" s="3"/>
       <c r="K381" s="3"/>
@@ -11912,7 +11907,7 @@
       <c r="E382" s="2"/>
       <c r="F382" s="2"/>
       <c r="G382" s="2"/>
-      <c r="H382" s="2"/>
+      <c r="H382" s="1"/>
       <c r="I382" s="3"/>
       <c r="J382" s="3"/>
       <c r="K382" s="3"/>
@@ -11942,7 +11937,7 @@
       <c r="E383" s="2"/>
       <c r="F383" s="2"/>
       <c r="G383" s="2"/>
-      <c r="H383" s="2"/>
+      <c r="H383" s="1"/>
       <c r="I383" s="3"/>
       <c r="J383" s="3"/>
       <c r="K383" s="3"/>
@@ -11972,7 +11967,7 @@
       <c r="E384" s="2"/>
       <c r="F384" s="2"/>
       <c r="G384" s="2"/>
-      <c r="H384" s="2"/>
+      <c r="H384" s="1"/>
       <c r="I384" s="3"/>
       <c r="J384" s="3"/>
       <c r="K384" s="3"/>
@@ -12002,7 +11997,7 @@
       <c r="E385" s="2"/>
       <c r="F385" s="2"/>
       <c r="G385" s="2"/>
-      <c r="H385" s="2"/>
+      <c r="H385" s="1"/>
       <c r="I385" s="3"/>
       <c r="J385" s="3"/>
       <c r="K385" s="3"/>
@@ -12032,7 +12027,7 @@
       <c r="E386" s="2"/>
       <c r="F386" s="2"/>
       <c r="G386" s="2"/>
-      <c r="H386" s="2"/>
+      <c r="H386" s="1"/>
       <c r="I386" s="3"/>
       <c r="J386" s="3"/>
       <c r="K386" s="3"/>
@@ -12062,7 +12057,7 @@
       <c r="E387" s="2"/>
       <c r="F387" s="2"/>
       <c r="G387" s="2"/>
-      <c r="H387" s="2"/>
+      <c r="H387" s="1"/>
       <c r="I387" s="3"/>
       <c r="J387" s="3"/>
       <c r="K387" s="3"/>
@@ -12092,7 +12087,7 @@
       <c r="E388" s="2"/>
       <c r="F388" s="2"/>
       <c r="G388" s="2"/>
-      <c r="H388" s="2"/>
+      <c r="H388" s="1"/>
       <c r="I388" s="3"/>
       <c r="J388" s="3"/>
       <c r="K388" s="3"/>
@@ -12122,7 +12117,7 @@
       <c r="E389" s="2"/>
       <c r="F389" s="2"/>
       <c r="G389" s="2"/>
-      <c r="H389" s="2"/>
+      <c r="H389" s="1"/>
       <c r="I389" s="3"/>
       <c r="J389" s="3"/>
       <c r="K389" s="3"/>
@@ -12152,7 +12147,7 @@
       <c r="E390" s="2"/>
       <c r="F390" s="2"/>
       <c r="G390" s="2"/>
-      <c r="H390" s="2"/>
+      <c r="H390" s="1"/>
       <c r="I390" s="3"/>
       <c r="J390" s="3"/>
       <c r="K390" s="3"/>
@@ -12182,7 +12177,7 @@
       <c r="E391" s="2"/>
       <c r="F391" s="2"/>
       <c r="G391" s="2"/>
-      <c r="H391" s="2"/>
+      <c r="H391" s="1"/>
       <c r="I391" s="3"/>
       <c r="J391" s="3"/>
       <c r="K391" s="3"/>
@@ -12212,7 +12207,7 @@
       <c r="E392" s="2"/>
       <c r="F392" s="2"/>
       <c r="G392" s="2"/>
-      <c r="H392" s="2"/>
+      <c r="H392" s="1"/>
       <c r="I392" s="3"/>
       <c r="J392" s="3"/>
       <c r="K392" s="3"/>
@@ -12242,7 +12237,7 @@
       <c r="E393" s="2"/>
       <c r="F393" s="2"/>
       <c r="G393" s="2"/>
-      <c r="H393" s="2"/>
+      <c r="H393" s="1"/>
       <c r="I393" s="3"/>
       <c r="J393" s="3"/>
       <c r="K393" s="3"/>
@@ -12272,7 +12267,7 @@
       <c r="E394" s="2"/>
       <c r="F394" s="2"/>
       <c r="G394" s="2"/>
-      <c r="H394" s="2"/>
+      <c r="H394" s="1"/>
       <c r="I394" s="3"/>
       <c r="J394" s="3"/>
       <c r="K394" s="3"/>
@@ -12302,7 +12297,7 @@
       <c r="E395" s="2"/>
       <c r="F395" s="2"/>
       <c r="G395" s="2"/>
-      <c r="H395" s="2"/>
+      <c r="H395" s="1"/>
       <c r="I395" s="3"/>
       <c r="J395" s="3"/>
       <c r="K395" s="3"/>
@@ -12332,7 +12327,7 @@
       <c r="E396" s="2"/>
       <c r="F396" s="2"/>
       <c r="G396" s="2"/>
-      <c r="H396" s="2"/>
+      <c r="H396" s="1"/>
       <c r="I396" s="3"/>
       <c r="J396" s="3"/>
       <c r="K396" s="3"/>
@@ -12362,7 +12357,7 @@
       <c r="E397" s="2"/>
       <c r="F397" s="2"/>
       <c r="G397" s="2"/>
-      <c r="H397" s="2"/>
+      <c r="H397" s="1"/>
       <c r="I397" s="3"/>
       <c r="J397" s="3"/>
       <c r="K397" s="3"/>
@@ -12392,7 +12387,7 @@
       <c r="E398" s="2"/>
       <c r="F398" s="2"/>
       <c r="G398" s="2"/>
-      <c r="H398" s="2"/>
+      <c r="H398" s="1"/>
       <c r="I398" s="3"/>
       <c r="J398" s="3"/>
       <c r="K398" s="3"/>
@@ -12422,7 +12417,7 @@
       <c r="E399" s="2"/>
       <c r="F399" s="2"/>
       <c r="G399" s="2"/>
-      <c r="H399" s="2"/>
+      <c r="H399" s="1"/>
       <c r="I399" s="3"/>
       <c r="J399" s="3"/>
       <c r="K399" s="3"/>
@@ -12452,7 +12447,7 @@
       <c r="E400" s="2"/>
       <c r="F400" s="2"/>
       <c r="G400" s="2"/>
-      <c r="H400" s="2"/>
+      <c r="H400" s="1"/>
       <c r="I400" s="3"/>
       <c r="J400" s="3"/>
       <c r="K400" s="3"/>
@@ -12482,7 +12477,7 @@
       <c r="E401" s="2"/>
       <c r="F401" s="2"/>
       <c r="G401" s="2"/>
-      <c r="H401" s="2"/>
+      <c r="H401" s="1"/>
       <c r="I401" s="3"/>
       <c r="J401" s="3"/>
       <c r="K401" s="3"/>
@@ -12512,7 +12507,7 @@
       <c r="E402" s="2"/>
       <c r="F402" s="2"/>
       <c r="G402" s="2"/>
-      <c r="H402" s="2"/>
+      <c r="H402" s="1"/>
       <c r="I402" s="3"/>
       <c r="J402" s="3"/>
       <c r="K402" s="3"/>
@@ -12542,7 +12537,7 @@
       <c r="E403" s="2"/>
       <c r="F403" s="2"/>
       <c r="G403" s="2"/>
-      <c r="H403" s="2"/>
+      <c r="H403" s="1"/>
       <c r="I403" s="3"/>
       <c r="J403" s="3"/>
       <c r="K403" s="3"/>
@@ -12572,7 +12567,7 @@
       <c r="E404" s="2"/>
       <c r="F404" s="2"/>
       <c r="G404" s="2"/>
-      <c r="H404" s="2"/>
+      <c r="H404" s="1"/>
       <c r="I404" s="3"/>
       <c r="J404" s="3"/>
       <c r="K404" s="3"/>
@@ -12602,7 +12597,7 @@
       <c r="E405" s="2"/>
       <c r="F405" s="2"/>
       <c r="G405" s="2"/>
-      <c r="H405" s="2"/>
+      <c r="H405" s="1"/>
       <c r="I405" s="3"/>
       <c r="J405" s="3"/>
       <c r="K405" s="3"/>
@@ -12632,7 +12627,7 @@
       <c r="E406" s="2"/>
       <c r="F406" s="2"/>
       <c r="G406" s="2"/>
-      <c r="H406" s="2"/>
+      <c r="H406" s="1"/>
       <c r="I406" s="3"/>
       <c r="J406" s="3"/>
       <c r="K406" s="3"/>
@@ -12662,7 +12657,7 @@
       <c r="E407" s="2"/>
       <c r="F407" s="2"/>
       <c r="G407" s="2"/>
-      <c r="H407" s="2"/>
+      <c r="H407" s="1"/>
       <c r="I407" s="3"/>
       <c r="J407" s="3"/>
       <c r="K407" s="3"/>
@@ -12692,7 +12687,7 @@
       <c r="E408" s="2"/>
       <c r="F408" s="2"/>
       <c r="G408" s="2"/>
-      <c r="H408" s="2"/>
+      <c r="H408" s="1"/>
       <c r="I408" s="3"/>
       <c r="J408" s="3"/>
       <c r="K408" s="3"/>
@@ -12722,7 +12717,7 @@
       <c r="E409" s="2"/>
       <c r="F409" s="2"/>
       <c r="G409" s="2"/>
-      <c r="H409" s="2"/>
+      <c r="H409" s="1"/>
       <c r="I409" s="3"/>
       <c r="J409" s="3"/>
       <c r="K409" s="3"/>
@@ -12752,7 +12747,7 @@
       <c r="E410" s="2"/>
       <c r="F410" s="2"/>
       <c r="G410" s="2"/>
-      <c r="H410" s="2"/>
+      <c r="H410" s="1"/>
       <c r="I410" s="3"/>
       <c r="J410" s="3"/>
       <c r="K410" s="3"/>
@@ -12782,7 +12777,7 @@
       <c r="E411" s="2"/>
       <c r="F411" s="2"/>
       <c r="G411" s="2"/>
-      <c r="H411" s="2"/>
+      <c r="H411" s="1"/>
       <c r="I411" s="3"/>
       <c r="J411" s="3"/>
       <c r="K411" s="3"/>
@@ -12812,7 +12807,7 @@
       <c r="E412" s="2"/>
       <c r="F412" s="2"/>
       <c r="G412" s="2"/>
-      <c r="H412" s="2"/>
+      <c r="H412" s="1"/>
       <c r="I412" s="3"/>
       <c r="J412" s="3"/>
       <c r="K412" s="3"/>
@@ -12842,7 +12837,7 @@
       <c r="E413" s="2"/>
       <c r="F413" s="2"/>
       <c r="G413" s="2"/>
-      <c r="H413" s="2"/>
+      <c r="H413" s="1"/>
       <c r="I413" s="3"/>
       <c r="J413" s="3"/>
       <c r="K413" s="3"/>
@@ -12872,7 +12867,7 @@
       <c r="E414" s="2"/>
       <c r="F414" s="2"/>
       <c r="G414" s="2"/>
-      <c r="H414" s="2"/>
+      <c r="H414" s="1"/>
       <c r="I414" s="3"/>
       <c r="J414" s="3"/>
       <c r="K414" s="3"/>
@@ -12902,7 +12897,7 @@
       <c r="E415" s="2"/>
       <c r="F415" s="2"/>
       <c r="G415" s="2"/>
-      <c r="H415" s="2"/>
+      <c r="H415" s="1"/>
       <c r="I415" s="3"/>
       <c r="J415" s="3"/>
       <c r="K415" s="3"/>
@@ -12932,7 +12927,7 @@
       <c r="E416" s="2"/>
       <c r="F416" s="2"/>
       <c r="G416" s="2"/>
-      <c r="H416" s="2"/>
+      <c r="H416" s="1"/>
       <c r="I416" s="3"/>
       <c r="J416" s="3"/>
       <c r="K416" s="3"/>
@@ -12962,7 +12957,7 @@
       <c r="E417" s="2"/>
       <c r="F417" s="2"/>
       <c r="G417" s="2"/>
-      <c r="H417" s="2"/>
+      <c r="H417" s="1"/>
       <c r="I417" s="3"/>
       <c r="J417" s="3"/>
       <c r="K417" s="3"/>
@@ -12992,7 +12987,7 @@
       <c r="E418" s="2"/>
       <c r="F418" s="2"/>
       <c r="G418" s="2"/>
-      <c r="H418" s="2"/>
+      <c r="H418" s="1"/>
       <c r="I418" s="3"/>
       <c r="J418" s="3"/>
       <c r="K418" s="3"/>
@@ -13022,7 +13017,7 @@
       <c r="E419" s="2"/>
       <c r="F419" s="2"/>
       <c r="G419" s="2"/>
-      <c r="H419" s="2"/>
+      <c r="H419" s="1"/>
       <c r="I419" s="3"/>
       <c r="J419" s="3"/>
       <c r="K419" s="3"/>
@@ -13052,7 +13047,7 @@
       <c r="E420" s="2"/>
       <c r="F420" s="2"/>
       <c r="G420" s="2"/>
-      <c r="H420" s="2"/>
+      <c r="H420" s="1"/>
       <c r="I420" s="3"/>
       <c r="J420" s="3"/>
       <c r="K420" s="3"/>
@@ -13082,7 +13077,7 @@
       <c r="E421" s="2"/>
       <c r="F421" s="2"/>
       <c r="G421" s="2"/>
-      <c r="H421" s="2"/>
+      <c r="H421" s="1"/>
       <c r="I421" s="3"/>
       <c r="J421" s="3"/>
       <c r="K421" s="3"/>
@@ -13112,7 +13107,7 @@
       <c r="E422" s="2"/>
       <c r="F422" s="2"/>
       <c r="G422" s="2"/>
-      <c r="H422" s="2"/>
+      <c r="H422" s="1"/>
       <c r="I422" s="3"/>
       <c r="J422" s="3"/>
       <c r="K422" s="3"/>
@@ -13142,7 +13137,7 @@
       <c r="E423" s="2"/>
       <c r="F423" s="2"/>
       <c r="G423" s="2"/>
-      <c r="H423" s="2"/>
+      <c r="H423" s="1"/>
       <c r="I423" s="3"/>
       <c r="J423" s="3"/>
       <c r="K423" s="3"/>
@@ -13172,7 +13167,7 @@
       <c r="E424" s="2"/>
       <c r="F424" s="2"/>
       <c r="G424" s="2"/>
-      <c r="H424" s="2"/>
+      <c r="H424" s="1"/>
       <c r="I424" s="3"/>
       <c r="J424" s="3"/>
       <c r="K424" s="3"/>
@@ -13202,7 +13197,7 @@
       <c r="E425" s="2"/>
       <c r="F425" s="2"/>
       <c r="G425" s="2"/>
-      <c r="H425" s="2"/>
+      <c r="H425" s="1"/>
       <c r="I425" s="3"/>
       <c r="J425" s="3"/>
       <c r="K425" s="3"/>
@@ -13232,7 +13227,7 @@
       <c r="E426" s="2"/>
       <c r="F426" s="2"/>
       <c r="G426" s="2"/>
-      <c r="H426" s="2"/>
+      <c r="H426" s="1"/>
       <c r="I426" s="3"/>
       <c r="J426" s="3"/>
       <c r="K426" s="3"/>
@@ -13262,7 +13257,7 @@
       <c r="E427" s="2"/>
       <c r="F427" s="2"/>
       <c r="G427" s="2"/>
-      <c r="H427" s="2"/>
+      <c r="H427" s="1"/>
       <c r="I427" s="3"/>
       <c r="J427" s="3"/>
       <c r="K427" s="3"/>
@@ -13292,7 +13287,7 @@
       <c r="E428" s="2"/>
       <c r="F428" s="2"/>
       <c r="G428" s="2"/>
-      <c r="H428" s="2"/>
+      <c r="H428" s="1"/>
       <c r="I428" s="3"/>
       <c r="J428" s="3"/>
       <c r="K428" s="3"/>
@@ -13322,7 +13317,7 @@
       <c r="E429" s="2"/>
       <c r="F429" s="2"/>
       <c r="G429" s="2"/>
-      <c r="H429" s="2"/>
+      <c r="H429" s="1"/>
       <c r="I429" s="3"/>
       <c r="J429" s="3"/>
       <c r="K429" s="3"/>
@@ -13352,7 +13347,7 @@
       <c r="E430" s="2"/>
       <c r="F430" s="2"/>
       <c r="G430" s="2"/>
-      <c r="H430" s="2"/>
+      <c r="H430" s="1"/>
       <c r="I430" s="3"/>
       <c r="J430" s="3"/>
       <c r="K430" s="3"/>
@@ -13382,7 +13377,7 @@
       <c r="E431" s="2"/>
       <c r="F431" s="2"/>
       <c r="G431" s="2"/>
-      <c r="H431" s="2"/>
+      <c r="H431" s="1"/>
       <c r="I431" s="3"/>
       <c r="J431" s="3"/>
       <c r="K431" s="3"/>
@@ -13412,7 +13407,7 @@
       <c r="E432" s="2"/>
       <c r="F432" s="2"/>
       <c r="G432" s="2"/>
-      <c r="H432" s="2"/>
+      <c r="H432" s="1"/>
       <c r="I432" s="3"/>
       <c r="J432" s="3"/>
       <c r="K432" s="3"/>
@@ -13442,7 +13437,7 @@
       <c r="E433" s="2"/>
       <c r="F433" s="2"/>
       <c r="G433" s="2"/>
-      <c r="H433" s="2"/>
+      <c r="H433" s="1"/>
       <c r="I433" s="3"/>
       <c r="J433" s="3"/>
       <c r="K433" s="3"/>
@@ -13472,7 +13467,7 @@
       <c r="E434" s="2"/>
       <c r="F434" s="2"/>
       <c r="G434" s="2"/>
-      <c r="H434" s="2"/>
+      <c r="H434" s="1"/>
       <c r="I434" s="3"/>
       <c r="J434" s="3"/>
       <c r="K434" s="3"/>
@@ -13502,7 +13497,7 @@
       <c r="E435" s="2"/>
       <c r="F435" s="2"/>
       <c r="G435" s="2"/>
-      <c r="H435" s="2"/>
+      <c r="H435" s="1"/>
       <c r="I435" s="3"/>
       <c r="J435" s="3"/>
       <c r="K435" s="3"/>
@@ -13532,7 +13527,7 @@
       <c r="E436" s="2"/>
       <c r="F436" s="2"/>
       <c r="G436" s="2"/>
-      <c r="H436" s="2"/>
+      <c r="H436" s="1"/>
       <c r="I436" s="3"/>
       <c r="J436" s="3"/>
       <c r="K436" s="3"/>
@@ -13562,7 +13557,7 @@
       <c r="E437" s="2"/>
       <c r="F437" s="2"/>
       <c r="G437" s="2"/>
-      <c r="H437" s="2"/>
+      <c r="H437" s="1"/>
       <c r="I437" s="3"/>
       <c r="J437" s="3"/>
       <c r="K437" s="3"/>
@@ -13592,7 +13587,7 @@
       <c r="E438" s="2"/>
       <c r="F438" s="2"/>
       <c r="G438" s="2"/>
-      <c r="H438" s="2"/>
+      <c r="H438" s="1"/>
       <c r="I438" s="3"/>
       <c r="J438" s="3"/>
       <c r="K438" s="3"/>
@@ -13622,7 +13617,7 @@
       <c r="E439" s="2"/>
       <c r="F439" s="2"/>
       <c r="G439" s="2"/>
-      <c r="H439" s="2"/>
+      <c r="H439" s="1"/>
       <c r="I439" s="3"/>
       <c r="J439" s="3"/>
       <c r="K439" s="3"/>
@@ -13652,7 +13647,7 @@
       <c r="E440" s="2"/>
       <c r="F440" s="2"/>
       <c r="G440" s="2"/>
-      <c r="H440" s="2"/>
+      <c r="H440" s="1"/>
       <c r="I440" s="3"/>
       <c r="J440" s="3"/>
       <c r="K440" s="3"/>
@@ -13682,7 +13677,7 @@
       <c r="E441" s="2"/>
       <c r="F441" s="2"/>
       <c r="G441" s="2"/>
-      <c r="H441" s="2"/>
+      <c r="H441" s="1"/>
       <c r="I441" s="3"/>
       <c r="J441" s="3"/>
       <c r="K441" s="3"/>
@@ -13712,7 +13707,7 @@
       <c r="E442" s="2"/>
       <c r="F442" s="2"/>
       <c r="G442" s="2"/>
-      <c r="H442" s="2"/>
+      <c r="H442" s="1"/>
       <c r="I442" s="3"/>
       <c r="J442" s="3"/>
       <c r="K442" s="3"/>
@@ -13742,7 +13737,7 @@
       <c r="E443" s="2"/>
       <c r="F443" s="2"/>
       <c r="G443" s="2"/>
-      <c r="H443" s="2"/>
+      <c r="H443" s="1"/>
       <c r="I443" s="3"/>
       <c r="J443" s="3"/>
       <c r="K443" s="3"/>
@@ -13772,7 +13767,7 @@
       <c r="E444" s="2"/>
       <c r="F444" s="2"/>
       <c r="G444" s="2"/>
-      <c r="H444" s="2"/>
+      <c r="H444" s="1"/>
       <c r="I444" s="3"/>
       <c r="J444" s="3"/>
       <c r="K444" s="3"/>
@@ -13802,7 +13797,7 @@
       <c r="E445" s="2"/>
       <c r="F445" s="2"/>
       <c r="G445" s="2"/>
-      <c r="H445" s="2"/>
+      <c r="H445" s="1"/>
     </row>
     <row r="446" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A446" s="2"/>
@@ -13812,7 +13807,7 @@
       <c r="E446" s="2"/>
       <c r="F446" s="2"/>
       <c r="G446" s="2"/>
-      <c r="H446" s="2"/>
+      <c r="H446" s="1"/>
     </row>
     <row r="447" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A447" s="2"/>
@@ -13822,7 +13817,7 @@
       <c r="E447" s="2"/>
       <c r="F447" s="2"/>
       <c r="G447" s="2"/>
-      <c r="H447" s="2"/>
+      <c r="H447" s="1"/>
     </row>
     <row r="448" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A448" s="2"/>
@@ -13832,7 +13827,7 @@
       <c r="E448" s="2"/>
       <c r="F448" s="2"/>
       <c r="G448" s="2"/>
-      <c r="H448" s="2"/>
+      <c r="H448" s="1"/>
     </row>
     <row r="449" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A449" s="2"/>
@@ -13842,7 +13837,7 @@
       <c r="E449" s="2"/>
       <c r="F449" s="2"/>
       <c r="G449" s="2"/>
-      <c r="H449" s="2"/>
+      <c r="H449" s="1"/>
     </row>
     <row r="450" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A450" s="2"/>
@@ -13852,7 +13847,7 @@
       <c r="E450" s="2"/>
       <c r="F450" s="2"/>
       <c r="G450" s="2"/>
-      <c r="H450" s="2"/>
+      <c r="H450" s="1"/>
     </row>
     <row r="451" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A451" s="2"/>
@@ -13862,7 +13857,7 @@
       <c r="E451" s="2"/>
       <c r="F451" s="2"/>
       <c r="G451" s="2"/>
-      <c r="H451" s="2"/>
+      <c r="H451" s="1"/>
     </row>
     <row r="452" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A452" s="2"/>
@@ -13872,7 +13867,7 @@
       <c r="E452" s="2"/>
       <c r="F452" s="2"/>
       <c r="G452" s="2"/>
-      <c r="H452" s="2"/>
+      <c r="H452" s="1"/>
     </row>
     <row r="453" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A453" s="2"/>
@@ -13882,7 +13877,7 @@
       <c r="E453" s="2"/>
       <c r="F453" s="2"/>
       <c r="G453" s="2"/>
-      <c r="H453" s="2"/>
+      <c r="H453" s="1"/>
     </row>
     <row r="454" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A454" s="2"/>
@@ -13892,7 +13887,7 @@
       <c r="E454" s="2"/>
       <c r="F454" s="2"/>
       <c r="G454" s="2"/>
-      <c r="H454" s="2"/>
+      <c r="H454" s="1"/>
     </row>
     <row r="455" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A455" s="2"/>
@@ -13902,7 +13897,7 @@
       <c r="E455" s="2"/>
       <c r="F455" s="2"/>
       <c r="G455" s="2"/>
-      <c r="H455" s="2"/>
+      <c r="H455" s="1"/>
     </row>
     <row r="456" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A456" s="2"/>
@@ -13912,7 +13907,7 @@
       <c r="E456" s="2"/>
       <c r="F456" s="2"/>
       <c r="G456" s="2"/>
-      <c r="H456" s="2"/>
+      <c r="H456" s="1"/>
     </row>
     <row r="457" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A457" s="2"/>
@@ -13922,7 +13917,7 @@
       <c r="E457" s="2"/>
       <c r="F457" s="2"/>
       <c r="G457" s="2"/>
-      <c r="H457" s="2"/>
+      <c r="H457" s="1"/>
     </row>
     <row r="458" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A458" s="2"/>
@@ -13932,7 +13927,7 @@
       <c r="E458" s="2"/>
       <c r="F458" s="2"/>
       <c r="G458" s="2"/>
-      <c r="H458" s="2"/>
+      <c r="H458" s="1"/>
     </row>
     <row r="459" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A459" s="2"/>
@@ -13942,7 +13937,7 @@
       <c r="E459" s="2"/>
       <c r="F459" s="2"/>
       <c r="G459" s="2"/>
-      <c r="H459" s="2"/>
+      <c r="H459" s="1"/>
     </row>
     <row r="460" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A460" s="2"/>
@@ -13952,7 +13947,7 @@
       <c r="E460" s="2"/>
       <c r="F460" s="2"/>
       <c r="G460" s="2"/>
-      <c r="H460" s="2"/>
+      <c r="H460" s="1"/>
     </row>
     <row r="461" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A461" s="2"/>
@@ -13962,7 +13957,7 @@
       <c r="E461" s="2"/>
       <c r="F461" s="2"/>
       <c r="G461" s="2"/>
-      <c r="H461" s="2"/>
+      <c r="H461" s="1"/>
     </row>
     <row r="462" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A462" s="2"/>
@@ -13972,7 +13967,7 @@
       <c r="E462" s="2"/>
       <c r="F462" s="2"/>
       <c r="G462" s="2"/>
-      <c r="H462" s="2"/>
+      <c r="H462" s="1"/>
     </row>
     <row r="463" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A463" s="2"/>
@@ -13982,7 +13977,7 @@
       <c r="E463" s="2"/>
       <c r="F463" s="2"/>
       <c r="G463" s="2"/>
-      <c r="H463" s="2"/>
+      <c r="H463" s="1"/>
     </row>
     <row r="464" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A464" s="2"/>
@@ -13992,7 +13987,7 @@
       <c r="E464" s="2"/>
       <c r="F464" s="2"/>
       <c r="G464" s="2"/>
-      <c r="H464" s="2"/>
+      <c r="H464" s="1"/>
     </row>
     <row r="465" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A465" s="2"/>
@@ -14002,7 +13997,7 @@
       <c r="E465" s="2"/>
       <c r="F465" s="2"/>
       <c r="G465" s="2"/>
-      <c r="H465" s="2"/>
+      <c r="H465" s="1"/>
     </row>
     <row r="466" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A466" s="2"/>
@@ -14012,7 +14007,7 @@
       <c r="E466" s="2"/>
       <c r="F466" s="2"/>
       <c r="G466" s="2"/>
-      <c r="H466" s="2"/>
+      <c r="H466" s="1"/>
     </row>
     <row r="467" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A467" s="2"/>
@@ -14022,7 +14017,7 @@
       <c r="E467" s="2"/>
       <c r="F467" s="2"/>
       <c r="G467" s="2"/>
-      <c r="H467" s="2"/>
+      <c r="H467" s="1"/>
     </row>
     <row r="468" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A468" s="2"/>
@@ -14032,7 +14027,7 @@
       <c r="E468" s="2"/>
       <c r="F468" s="2"/>
       <c r="G468" s="2"/>
-      <c r="H468" s="2"/>
+      <c r="H468" s="1"/>
     </row>
     <row r="469" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A469" s="2"/>
@@ -14042,7 +14037,7 @@
       <c r="E469" s="2"/>
       <c r="F469" s="2"/>
       <c r="G469" s="2"/>
-      <c r="H469" s="2"/>
+      <c r="H469" s="1"/>
     </row>
     <row r="470" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A470" s="2"/>
@@ -14052,7 +14047,7 @@
       <c r="E470" s="2"/>
       <c r="F470" s="2"/>
       <c r="G470" s="2"/>
-      <c r="H470" s="2"/>
+      <c r="H470" s="1"/>
     </row>
     <row r="471" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A471" s="2"/>
@@ -14062,7 +14057,7 @@
       <c r="E471" s="2"/>
       <c r="F471" s="2"/>
       <c r="G471" s="2"/>
-      <c r="H471" s="2"/>
+      <c r="H471" s="1"/>
     </row>
     <row r="472" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A472" s="2"/>
@@ -14072,7 +14067,7 @@
       <c r="E472" s="2"/>
       <c r="F472" s="2"/>
       <c r="G472" s="2"/>
-      <c r="H472" s="2"/>
+      <c r="H472" s="1"/>
     </row>
     <row r="473" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A473" s="2"/>
@@ -14082,7 +14077,7 @@
       <c r="E473" s="2"/>
       <c r="F473" s="2"/>
       <c r="G473" s="2"/>
-      <c r="H473" s="2"/>
+      <c r="H473" s="1"/>
     </row>
     <row r="474" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A474" s="2"/>
@@ -14092,7 +14087,7 @@
       <c r="E474" s="2"/>
       <c r="F474" s="2"/>
       <c r="G474" s="2"/>
-      <c r="H474" s="2"/>
+      <c r="H474" s="1"/>
     </row>
     <row r="475" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A475" s="2"/>
@@ -14102,7 +14097,7 @@
       <c r="E475" s="2"/>
       <c r="F475" s="2"/>
       <c r="G475" s="2"/>
-      <c r="H475" s="2"/>
+      <c r="H475" s="1"/>
     </row>
     <row r="476" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A476" s="2"/>
@@ -14112,7 +14107,7 @@
       <c r="E476" s="2"/>
       <c r="F476" s="2"/>
       <c r="G476" s="2"/>
-      <c r="H476" s="2"/>
+      <c r="H476" s="1"/>
     </row>
     <row r="477" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A477" s="2"/>
@@ -14122,7 +14117,7 @@
       <c r="E477" s="2"/>
       <c r="F477" s="2"/>
       <c r="G477" s="2"/>
-      <c r="H477" s="2"/>
+      <c r="H477" s="1"/>
     </row>
     <row r="478" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A478" s="2"/>
@@ -14132,7 +14127,7 @@
       <c r="E478" s="2"/>
       <c r="F478" s="2"/>
       <c r="G478" s="2"/>
-      <c r="H478" s="2"/>
+      <c r="H478" s="1"/>
     </row>
     <row r="479" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A479" s="2"/>
@@ -14142,7 +14137,7 @@
       <c r="E479" s="2"/>
       <c r="F479" s="2"/>
       <c r="G479" s="2"/>
-      <c r="H479" s="2"/>
+      <c r="H479" s="1"/>
     </row>
     <row r="480" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A480" s="2"/>
@@ -14152,7 +14147,7 @@
       <c r="E480" s="2"/>
       <c r="F480" s="2"/>
       <c r="G480" s="2"/>
-      <c r="H480" s="2"/>
+      <c r="H480" s="1"/>
     </row>
     <row r="481" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A481" s="2"/>
@@ -14162,7 +14157,7 @@
       <c r="E481" s="2"/>
       <c r="F481" s="2"/>
       <c r="G481" s="2"/>
-      <c r="H481" s="2"/>
+      <c r="H481" s="1"/>
     </row>
     <row r="482" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A482" s="2"/>
@@ -14172,7 +14167,7 @@
       <c r="E482" s="2"/>
       <c r="F482" s="2"/>
       <c r="G482" s="2"/>
-      <c r="H482" s="2"/>
+      <c r="H482" s="1"/>
     </row>
     <row r="483" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A483" s="2"/>
@@ -14182,7 +14177,7 @@
       <c r="E483" s="2"/>
       <c r="F483" s="2"/>
       <c r="G483" s="2"/>
-      <c r="H483" s="2"/>
+      <c r="H483" s="1"/>
     </row>
     <row r="484" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A484" s="2"/>
@@ -14192,7 +14187,7 @@
       <c r="E484" s="2"/>
       <c r="F484" s="2"/>
       <c r="G484" s="2"/>
-      <c r="H484" s="2"/>
+      <c r="H484" s="1"/>
     </row>
     <row r="485" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A485" s="2"/>
@@ -14202,7 +14197,7 @@
       <c r="E485" s="2"/>
       <c r="F485" s="2"/>
       <c r="G485" s="2"/>
-      <c r="H485" s="2"/>
+      <c r="H485" s="1"/>
     </row>
     <row r="486" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A486" s="2"/>
@@ -14212,7 +14207,7 @@
       <c r="E486" s="2"/>
       <c r="F486" s="2"/>
       <c r="G486" s="2"/>
-      <c r="H486" s="2"/>
+      <c r="H486" s="1"/>
     </row>
     <row r="487" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A487" s="2"/>
@@ -14222,7 +14217,7 @@
       <c r="E487" s="2"/>
       <c r="F487" s="2"/>
       <c r="G487" s="2"/>
-      <c r="H487" s="2"/>
+      <c r="H487" s="1"/>
     </row>
     <row r="488" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A488" s="2"/>
@@ -14232,7 +14227,7 @@
       <c r="E488" s="2"/>
       <c r="F488" s="2"/>
       <c r="G488" s="2"/>
-      <c r="H488" s="2"/>
+      <c r="H488" s="1"/>
     </row>
     <row r="489" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A489" s="2"/>
@@ -14242,7 +14237,7 @@
       <c r="E489" s="2"/>
       <c r="F489" s="2"/>
       <c r="G489" s="2"/>
-      <c r="H489" s="2"/>
+      <c r="H489" s="1"/>
     </row>
     <row r="490" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A490" s="2"/>
@@ -14252,7 +14247,7 @@
       <c r="E490" s="2"/>
       <c r="F490" s="2"/>
       <c r="G490" s="2"/>
-      <c r="H490" s="2"/>
+      <c r="H490" s="1"/>
     </row>
     <row r="491" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A491" s="2"/>
@@ -14262,7 +14257,7 @@
       <c r="E491" s="2"/>
       <c r="F491" s="2"/>
       <c r="G491" s="2"/>
-      <c r="H491" s="2"/>
+      <c r="H491" s="1"/>
     </row>
     <row r="492" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A492" s="2"/>
@@ -14272,7 +14267,7 @@
       <c r="E492" s="2"/>
       <c r="F492" s="2"/>
       <c r="G492" s="2"/>
-      <c r="H492" s="2"/>
+      <c r="H492" s="1"/>
     </row>
     <row r="493" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A493" s="2"/>
@@ -14282,7 +14277,7 @@
       <c r="E493" s="2"/>
       <c r="F493" s="2"/>
       <c r="G493" s="2"/>
-      <c r="H493" s="2"/>
+      <c r="H493" s="1"/>
     </row>
     <row r="494" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A494" s="2"/>
@@ -14292,7 +14287,7 @@
       <c r="E494" s="2"/>
       <c r="F494" s="2"/>
       <c r="G494" s="2"/>
-      <c r="H494" s="2"/>
+      <c r="H494" s="1"/>
     </row>
     <row r="495" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A495" s="2"/>
@@ -14302,7 +14297,7 @@
       <c r="E495" s="2"/>
       <c r="F495" s="2"/>
       <c r="G495" s="2"/>
-      <c r="H495" s="2"/>
+      <c r="H495" s="1"/>
     </row>
     <row r="496" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A496" s="2"/>
@@ -14312,7 +14307,7 @@
       <c r="E496" s="2"/>
       <c r="F496" s="2"/>
       <c r="G496" s="2"/>
-      <c r="H496" s="2"/>
+      <c r="H496" s="1"/>
     </row>
     <row r="497" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A497" s="2"/>
@@ -14322,7 +14317,7 @@
       <c r="E497" s="2"/>
       <c r="F497" s="2"/>
       <c r="G497" s="2"/>
-      <c r="H497" s="2"/>
+      <c r="H497" s="1"/>
     </row>
     <row r="498" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A498" s="2"/>
@@ -14332,7 +14327,7 @@
       <c r="E498" s="2"/>
       <c r="F498" s="2"/>
       <c r="G498" s="2"/>
-      <c r="H498" s="2"/>
+      <c r="H498" s="1"/>
     </row>
     <row r="499" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A499" s="2"/>
@@ -14342,7 +14337,7 @@
       <c r="E499" s="2"/>
       <c r="F499" s="2"/>
       <c r="G499" s="2"/>
-      <c r="H499" s="2"/>
+      <c r="H499" s="1"/>
     </row>
     <row r="500" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A500" s="2"/>
@@ -14352,7 +14347,7 @@
       <c r="E500" s="2"/>
       <c r="F500" s="2"/>
       <c r="G500" s="2"/>
-      <c r="H500" s="2"/>
+      <c r="H500" s="1"/>
     </row>
     <row r="501" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A501" s="2"/>
@@ -14362,7 +14357,7 @@
       <c r="E501" s="2"/>
       <c r="F501" s="2"/>
       <c r="G501" s="2"/>
-      <c r="H501" s="2"/>
+      <c r="H501" s="1"/>
     </row>
     <row r="502" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A502" s="2"/>
@@ -14372,7 +14367,7 @@
       <c r="E502" s="2"/>
       <c r="F502" s="2"/>
       <c r="G502" s="2"/>
-      <c r="H502" s="2"/>
+      <c r="H502" s="1"/>
     </row>
     <row r="503" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A503" s="2"/>
@@ -14382,7 +14377,7 @@
       <c r="E503" s="2"/>
       <c r="F503" s="2"/>
       <c r="G503" s="2"/>
-      <c r="H503" s="2"/>
+      <c r="H503" s="1"/>
     </row>
     <row r="504" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A504" s="2"/>
@@ -14392,7 +14387,7 @@
       <c r="E504" s="2"/>
       <c r="F504" s="2"/>
       <c r="G504" s="2"/>
-      <c r="H504" s="2"/>
+      <c r="H504" s="1"/>
     </row>
     <row r="505" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A505" s="2"/>
@@ -14402,7 +14397,7 @@
       <c r="E505" s="2"/>
       <c r="F505" s="2"/>
       <c r="G505" s="2"/>
-      <c r="H505" s="2"/>
+      <c r="H505" s="1"/>
     </row>
     <row r="506" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A506" s="2"/>
@@ -14412,7 +14407,7 @@
       <c r="E506" s="2"/>
       <c r="F506" s="2"/>
       <c r="G506" s="2"/>
-      <c r="H506" s="2"/>
+      <c r="H506" s="1"/>
     </row>
     <row r="507" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A507" s="2"/>
@@ -14422,7 +14417,7 @@
       <c r="E507" s="2"/>
       <c r="F507" s="2"/>
       <c r="G507" s="2"/>
-      <c r="H507" s="2"/>
+      <c r="H507" s="1"/>
     </row>
     <row r="508" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A508" s="2"/>
@@ -14432,7 +14427,7 @@
       <c r="E508" s="2"/>
       <c r="F508" s="2"/>
       <c r="G508" s="2"/>
-      <c r="H508" s="2"/>
+      <c r="H508" s="1"/>
     </row>
     <row r="509" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A509" s="2"/>
@@ -14442,17 +14437,39 @@
       <c r="E509" s="2"/>
       <c r="F509" s="2"/>
       <c r="G509" s="2"/>
-      <c r="H509" s="2"/>
+      <c r="H509" s="1"/>
+    </row>
+    <row r="510" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C510" s="2"/>
+      <c r="D510" s="2"/>
+      <c r="H510" s="1"/>
+    </row>
+    <row r="511" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C511" s="2"/>
+      <c r="D511" s="2"/>
+      <c r="H511" s="1"/>
+    </row>
+    <row r="512" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C512" s="2"/>
+      <c r="D512" s="2"/>
+      <c r="H512" s="1"/>
+    </row>
+    <row r="513" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C513" s="2"/>
+      <c r="D513" s="2"/>
+    </row>
+    <row r="514" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="D514" s="2"/>
+    </row>
+    <row r="515" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="D515" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Por favor ingresa solo numeros" sqref="C2:C347 D2:D500" xr:uid="{BEB12ADA-3A90-4DDE-982F-5986AEF8544A}">
-      <formula1>0</formula1>
-    </dataValidation>
+  <dataValidations count="2">
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Debes ingresar solo numeros" sqref="F2:F506" xr:uid="{7A15190E-E856-46CC-9451-DC106F83F56B}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Debes ingresar solo numeros" sqref="H2:H507" xr:uid="{45AB8757-468E-4673-8316-1FCA11D0844B}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Por favor ingresa solo numeros" sqref="D2:D515 C2:C513" xr:uid="{97EFAC3B-C871-41E9-BA0B-57A37F6CF4CB}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -14464,13 +14481,13 @@
           <x14:formula1>
             <xm:f>Hoja2!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>G2 G4:G355 G3</xm:sqref>
+          <xm:sqref>G2:G355</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9A47EBC6-339D-433F-AE00-43D43D6B56F7}">
           <x14:formula1>
             <xm:f>Hoja2!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E503 E2</xm:sqref>
+          <xm:sqref>E2:E503</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -14490,18 +14507,18 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>